<commit_message>
🤖 Auto-scrape: 2026-02-25 — Guardian Life Jobs
</commit_message>
<xml_diff>
--- a/output/GuardianLife_Jobs_2026-02-25.xlsx
+++ b/output/GuardianLife_Jobs_2026-02-25.xlsx
@@ -1407,20 +1407,24 @@
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>Senior Engineer IT</t>
+          <t>Group Benefits HR Business/Talent Partner</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
         <is>
-          <t>Job Description: Job Description: We are seeking a skilled and experienced Insurance Domain Techno Automation Senior QE engineer to join our team. The ideal candidate will have a strong understanding of software testing methodologies coupled with expertise in insurance industry processes, and products. As a Senior Automation Engineer you will collaborate closely with business analysts, developers, and other stakeholders to ensure the quality and reliability of insurance software systems using manual and automation testing. Your responsibilities will include designing, executing, and documenting test cases, identifying defects, and verifying fixes. You will also participate in requirement analysis and support user acceptance testing. The role requires excellent communication skills, automation skills (selenium &amp; Java), attention to detail, and the ability to work effectively in a dynamic, fast-paced environment. Key Responsibilities: Collaborate with stakeholders to understand business requirements and functional specifications. Understand and create reusable utilities and libraries at the framework level. Understand the existing automation framework code and then build on top of it, as per the new enhancements. Understand the existing API automation framework and then build on top of it, as per the new enhancements. Integrate automated tests into CI/CD pipelines (e.g., Jenkins, GitLab CI, Azure DevOps). Design and execute test cases based on business requirements and user stories. Able to work on the testing of sprint stories and figure out regression test cases out of them, which can be automated. Identify, document, and track defects using appropriate tools and techniques. Verify defect fixes and ensure that software meets quality standards and acceptance criteria. Participate in requirement analysis and contribute to test planning and estimation activities. Support user acceptance testing and assist in troubleshooting issues reported by end-users. Continuously improve testing processes and methodologies to enhance efficiency and effectiveness. Proactive, Self-motivated and ability to work on his/her individual capacity. Effective reporting capabilities on daily/weekly status. Requirements: B.Tech/B.E in Computer Science, Information Technology, or related field/MCA. 3-6 years of experience in software testing, preferably in the insurance domain. Hand On experience in automation tools like Selenium (with Java), Rest Assured &amp; Postman is a must. Should be able to implement an automation solution wherever required. Experience with test management tools &amp; defect management tools like JIRA &amp; QTest. Solid knowledge of software testing methodologies, techniques, and best practices. Experience with XML and Database testing is a plus. Should have hands on experience in Mobile Testing. Understanding of insurance industry processes, products, and regulations is good to have. Familiarity with Agile/Scrum methodologies and tools such as JIRA. Excellent analytical and problem-solving skills with a keen attention to detail. Strong communication and interpersonal skills, with the ability to collaborate effectively with cross-functional teams. Relevant certifications such as ISTQB Foundation Level or equivalent, CSM, Safe agile are a plus. Location: This position can be based in any of the following locations: Chennai Current Guardian Colleagues: Please apply through the internal Jobs Hub in Workday</t>
+          <t>Guardian is seeking a Human Resources Talent Partner (HRTP) for our growing Group Benefits business. This is a strategic HR role that requires strong consultative skills to facilitate culture change and build leadership capability. This role requires the HRTP to execute many facets of the talent strategy, demonstrating the ability to solve problems, coach leaders through demanding situations and change, while tracking and assessing changes and progress in the organization. You will Partner with leaders and their teams to develop and execute a talent strategy that enables business growth, leadership development, succession planning, employee engagement, equity, and inclusion. Collaborate with leaders to identify areas to enhance business performance through strategy, structure, process, people, and rewards. Assist in design and implementation of retention strategies focusing on key leaders and individuals with core competencies or skills critical to the organization – now and for the future. Support the development of effective leaders within the organization, focusing on leadership needs and key themes identified as part of the business strategy and organizational and talent review processes. Play an active role in guiding leaders through ongoing talent review and succession planning activities. Collaborate with leaders to create strategies to close talent gaps, develop a highly effective leadership team and bench strength for succession. Encourage building organizational and talent strength through diversity. Partner with leaders on employee engagement using data to identify factors that drive performance, commitment, and intent to stay; partner with leaders to develop plans in support of improving engagement. Recommend solutions to improve processes, team dynamics, etc. to optimize organizational effectiveness. Execute and drive plans for organizational change initiatives including organizational design, communication plans, upskilling, training, and problem solving. Provide strategic and day-to-day HR consultation to business leaders. Coach leaders on their personal efficacy and leadership impact. Partner and coordinate with HR Center of Excellence (COE) resources to identify requirements and execute actions in support of building talent and capabilities across assigned functional areas. Maintain an effective level of business literacy to be able to substantively contribute to the success of the business. Serve as a contributing member of Guardian HR community, playing a key role in driving key HR processes and initiatives within respective client groups. Participate as a member of project teams on enterprise-wide organizational HR initiatives. You have Business Acumen 10 plus years of human resources experience with solid business acumen and ability to create and implement human capital initiatives that enable the business strategy. The ability to work effectively within the organization’s financial and operational context. Demonstrated financial and analytical acumen to synthesize and prioritize ranging issues and activities, thus be highly effective in formulating coordinated action plans and activities. Data Judgment Experience leveraging data to influence decision making outcomes with ability to “tell the story “By utilizing data. Demonstrated strong analytical and assessment skills. Strategic Thinking The ability to develop and execute solutions to business challenges and to influence strategic business decisions. Strategic Human Resource Thought Leadership – can execute HR strategies across the organization in an efficient manner. Relationship Management/ Collaboration Ability to build relationships and quickly earn the trust of leaders, partners, key stakeholders, and collaborators, building credibility and becoming their trusted advisor. Proven experience in driving change, negotiating, and influencing leaders and key stakeholders across levels. Demonstrated courage to make difficult decisions by establishing high trust and credibility with the business leaders. Talent Management Demonstrated expertise in business and talent strategy, culture change, workforce planning, data and analytics, organizational design, talent management, and transformational organizational changes. The ability to identify, support and execute HR activities of strategic value to the organization and meet employees' needs across the employee life cycle. The ability to inspire employees at all levels and drive the talent agenda forward. Agility The ability to respond to shifts in the business environment and to adapt and change course when necessary. The ability to use excellent judgment while working with multiple priorities and deadlines in a fast-paced environment. Intellectual curiosity brings insights into the team and business with continual willingness to learn. Proven ability to foster change, influence leadership and build relationships with all colleague levels and be regarded as a trusted partner. Additionally BA/BS or equivalent work experience required in Human Resources or related field. Excellent verbal and written communication skills for multiple audiences including staff, management, and senior executives. Proven project leader experience in a highly matrixed organization working across multiple business lines. High degree of self-motivation, demonstrating initiative and an ability to manage multiple priorities with a sense of urgency and results orientation. Detail oriented mindset with a disciplined approach to process. Experience in Workday (preferred). Location /Travel Hybrid role –in office 3 days a week, Boston, MA; Hudson Yards, NYC; Stamford CT; or Bethlehem, PA. 2 days WFH Travel to other Guardian offices as needed – up to 15%. Salary Range: $132,420.00 - $217,545.00 The salary range reflected above is a good faith estimate of base pay for the primary location of the position. The salary for this position ultimately will be determined based on the education, experience, knowledge, and abilities of the successful candidate. In addition to salary, this role may also be eligible for annual, sales, or other incentive compensation. Our Promise At Guardian, you’ll have the support and flexibility to achieve your professional and personal goals.  Through skill-building, leadership development and philanthropic opportunities, we provide opportunities to build communities and grow your career, surrounded by diverse colleagues with high ethical standards. Inspire Well-Being As part of Guardian’s Purpose – to inspire well-being – we are committed to offering contemporary, supportive, flexible, and inclusive benefits and resources to our colleagues. Explore our company benefits at www.guardianlife.com/careers/corporate/benefits . Benefits apply to full-time eligible employees. Interns are not eligible for most Company benefits. Equal Employment Opportunity Guardian is an equal opportunity employer. All qualified applicants will be considered for employment without regard to age, race, color, creed, religion, sex, affectional or sexual orientation, national origin, ancestry, marital status, disability, military or veteran status, or any other classification protected by applicable law. Accommodations Guardian is committed to providing access, equal opportunity and reasonable accommodation for individuals with disabilities in employment, its services, programs, and activities. Guardian also provides reasonable accommodations to qualified job applicants (and employees) to accommodate the individual's known limitations related to pregnancy, childbirth, or related medical conditions, unless doing so would create an undue hardship. If reasonable accommodation is needed to participate in the job application or interview process, to perform essential job functions, and/or to receive other benefits and privileges of employment, please contact MyHR@glic.com. Please note: this resource is for accommodation requests only. For all other inquires related to your application and careers at Guardian, refer to the Guardian Careers site. Visa Sponsorship Guardian is not currently or in the foreseeable future sponsoring employment visas.  In order to be a successful applicant. you must be legally authorized to work in the United States, without the need for employer sponsorship. Current Guardian Colleagues: Please apply through the internal Jobs Hub in Workday.</t>
         </is>
       </c>
       <c r="D22" s="3" t="inlineStr">
         <is>
-          <t>Chennai</t>
-        </is>
-      </c>
-      <c r="E22" s="3" t="inlineStr"/>
+          <t>Boston</t>
+        </is>
+      </c>
+      <c r="E22" s="3" t="inlineStr">
+        <is>
+          <t>Bethlehem, New York, Stamford</t>
+        </is>
+      </c>
       <c r="F22" s="3" t="inlineStr">
         <is>
           <t>2026-02-17</t>
@@ -1428,13 +1432,17 @@
       </c>
       <c r="G22" s="3" t="inlineStr">
         <is>
-          <t>R000108657</t>
-        </is>
-      </c>
-      <c r="H22" s="3" t="inlineStr"/>
+          <t>R000108679</t>
+        </is>
+      </c>
+      <c r="H22" s="3" t="inlineStr">
+        <is>
+          <t>Hybrid - In office 3 days per week</t>
+        </is>
+      </c>
       <c r="I22" s="3" t="inlineStr">
         <is>
-          <t>https://guardianlife.wd5.myworkdayjobs.com/Guardian-Life-Careers/job/Chennai/Senior-Engineer-IT_R000108657-1</t>
+          <t>https://guardianlife.wd5.myworkdayjobs.com/Guardian-Life-Careers/job/Boston/Group-Benefits-HR-Business-Talent-Partner_R000108679-1</t>
         </is>
       </c>
     </row>
@@ -1446,42 +1454,34 @@
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t>Lead, Cybersecurity Assurance Testing</t>
+          <t>Senior Engineer IT</t>
         </is>
       </c>
       <c r="C23" s="4" t="inlineStr">
         <is>
-          <t>Lead, Cyber Security Assurance Testing The Lead, Cyber Security Assurance Testing is a working‑lead / “player‑coach role” within Guardian’s Cybersecurity Assurance organization. This role includes formal people management responsibility for a small number of senior engineers, with a focus on operational and tactical planning ,execution, and reporting, contributing to strategic planning, and accountable for project and program outcomes. The role is structured roughly as: ~60% leadership, coordination, and program execution ~40% hands‑on technical contribution and research This position leads through influence, technical credibility, and ownership. It is designed for an experienced security professional who demonstrates ambition, strong execution discipline, and the potential to grow into broader leadership over time, while remaining close to the work today. The role supports and helps evolve Guardian’s Application Security Testing, Ethical Hacking (Red Team), and Third‑Party Testing programs, working closely with Cyber Defense, application owners, and Guardian India Security Assurance. Key Responsibilities Lead and coordinate day ‑ to ‑ day execution of: Application Security Testing Ethical Hacking / Red Team activities Third‑party penetration testing engagements Lead the Improvement and evolution of AppSec and Red Team programs, increasing consistency, structure, and measurable outcomes. Own and maintain processes, procedures, playbooks, and documentation to ensure clarity, repeatability, and quality. Contribute to and execute against program planning artifacts, including Roadmaps, backlogs, and quarterly and annual goals Coordinate work across US And India Based assurance staff and third party testing vendors. Remain actively involved in application security testing and ethical hacking, providing technical guidance and quality assurance Participate selectively in: Targeted application security testing Rating &amp; Validation of high‑risk or high‑impact findings Red‑team or adversarial exercises where appropriate Provide technical review and direction: Support security product evaluation, selection, proof‑of‑concepts, and implementation, ensuring tools are operationalized effectively. Communicate technical findings clearly and simply to non‑technical stakeholders. Translate testing results into risk‑based, actionable insights. Collaborate closely with Cyber Defense, application teams, and security stakeholders to ensure testing results lead to defensive improvements and remediation. Required Qualifications 5+ years of experience in application security testing, ethical hacking, or offensive security, with demonstrated leadership responsibility. Strong understanding of: Application security testing techniques Penetration testing vs. red team objectives Secure SDLC and risk-based testing Hands on technical experience validating vulnerabilities and testing application security controls. Experience improving or evolving existing security programs, rather than only building from scratch. Strong process orientation with proven ability to create practical, lightweight documentation. Excellent communication skills with the ability to explain technical concepts in simple, business relevant terms. Demonstrated ambition and intent to grow into broader leadership scope over time. Bachelor’s degree in a related field or equivalent experience/certifications. Preferred Qualifications Experience in financial services or other large, regulated enterprise environments. Exposure to cloud‑native application security and modern CI/CD environments. Experience working with globally distributed teams (e.g., US and India). Familiarity with AppSec and Offensive Security tools. Location Three days a week at our Guardian office in New York, NY or Bethlehem, PA Salary Range: $118,980.00 - $195,465.00 The salary range reflected above is a good faith estimate of base pay for the primary location of the position. The salary for this position ultimately will be determined based on the education, experience, knowledge, and abilities of the successful candidate. In addition to salary, this role may also be eligible for annual, sales, or other incentive compensation. Our Promise At Guardian, you’ll have the support and flexibility to achieve your professional and personal goals.  Through skill-building, leadership development and philanthropic opportunities, we provide opportunities to build communities and grow your career, surrounded by diverse colleagues with high ethical standards. Inspire Well-Being As part of Guardian’s Purpose – to inspire well-being – we are committed to offering contemporary, supportive, flexible, and inclusive benefits and resources to our colleagues. Explore our company benefits at www.guardianlife.com/careers/corporate/benefits . Benefits apply to full-time eligible employees. Interns are not eligible for most Company benefits. Equal Employment Opportunity Guardian is an equal opportunity employer. All qualified applicants will be considered for employment without regard to age, race, color, creed, religion, sex, affectional or sexual orientation, national origin, ancestry, marital status, disability, military or veteran status, or any other classification protected by applicable law. Accommodations Guardian is committed to providing access, equal opportunity and reasonable accommodation for individuals with disabilities in employment, its services, programs, and activities. Guardian also provides reasonable accommodations to qualified job applicants (and employees) to accommodate the individual's known limitations related to pregnancy, childbirth, or related medical conditions, unless doing so would create an undue hardship. If reasonable accommodation is needed to participate in the job application or interview process, to perform essential job functions, and/or to receive other benefits and privileges of employment, please contact MyHR@glic.com. Please note: this resource is for accommodation requests only. For all other inquires related to your application and careers at Guardian, refer to the Guardian Careers site. Visa Sponsorship Guardian is not currently or in the foreseeable future sponsoring employment visas.  In order to be a successful applicant. you must be legally authorized to work in the United States, without the need for employer sponsorship. Current Guardian Colleagues: Please apply through the internal Jobs Hub in Workday.</t>
+          <t>Job Description: Job Description: We are seeking a skilled and experienced Insurance Domain Techno Automation Senior QE engineer to join our team. The ideal candidate will have a strong understanding of software testing methodologies coupled with expertise in insurance industry processes, and products. As a Senior Automation Engineer you will collaborate closely with business analysts, developers, and other stakeholders to ensure the quality and reliability of insurance software systems using manual and automation testing. Your responsibilities will include designing, executing, and documenting test cases, identifying defects, and verifying fixes. You will also participate in requirement analysis and support user acceptance testing. The role requires excellent communication skills, automation skills (selenium &amp; Java), attention to detail, and the ability to work effectively in a dynamic, fast-paced environment. Key Responsibilities: Collaborate with stakeholders to understand business requirements and functional specifications. Understand and create reusable utilities and libraries at the framework level. Understand the existing automation framework code and then build on top of it, as per the new enhancements. Understand the existing API automation framework and then build on top of it, as per the new enhancements. Integrate automated tests into CI/CD pipelines (e.g., Jenkins, GitLab CI, Azure DevOps). Design and execute test cases based on business requirements and user stories. Able to work on the testing of sprint stories and figure out regression test cases out of them, which can be automated. Identify, document, and track defects using appropriate tools and techniques. Verify defect fixes and ensure that software meets quality standards and acceptance criteria. Participate in requirement analysis and contribute to test planning and estimation activities. Support user acceptance testing and assist in troubleshooting issues reported by end-users. Continuously improve testing processes and methodologies to enhance efficiency and effectiveness. Proactive, Self-motivated and ability to work on his/her individual capacity. Effective reporting capabilities on daily/weekly status. Requirements: B.Tech/B.E in Computer Science, Information Technology, or related field/MCA. 3-6 years of experience in software testing, preferably in the insurance domain. Hand On experience in automation tools like Selenium (with Java), Rest Assured &amp; Postman is a must. Should be able to implement an automation solution wherever required. Experience with test management tools &amp; defect management tools like JIRA &amp; QTest. Solid knowledge of software testing methodologies, techniques, and best practices. Experience with XML and Database testing is a plus. Should have hands on experience in Mobile Testing. Understanding of insurance industry processes, products, and regulations is good to have. Familiarity with Agile/Scrum methodologies and tools such as JIRA. Excellent analytical and problem-solving skills with a keen attention to detail. Strong communication and interpersonal skills, with the ability to collaborate effectively with cross-functional teams. Relevant certifications such as ISTQB Foundation Level or equivalent, CSM, Safe agile are a plus. Location: This position can be based in any of the following locations: Chennai Current Guardian Colleagues: Please apply through the internal Jobs Hub in Workday</t>
         </is>
       </c>
       <c r="D23" s="4" t="inlineStr">
         <is>
-          <t>New York</t>
-        </is>
-      </c>
-      <c r="E23" s="4" t="inlineStr">
-        <is>
-          <t>Bethlehem</t>
-        </is>
-      </c>
+          <t>Chennai</t>
+        </is>
+      </c>
+      <c r="E23" s="4" t="inlineStr"/>
       <c r="F23" s="4" t="inlineStr">
         <is>
-          <t>2026-02-13</t>
+          <t>2026-02-17</t>
         </is>
       </c>
       <c r="G23" s="4" t="inlineStr">
         <is>
-          <t>R000108255</t>
-        </is>
-      </c>
-      <c r="H23" s="4" t="inlineStr">
-        <is>
-          <t>Hybrid - In office 3 days per week</t>
-        </is>
-      </c>
+          <t>R000108657</t>
+        </is>
+      </c>
+      <c r="H23" s="4" t="inlineStr"/>
       <c r="I23" s="4" t="inlineStr">
         <is>
-          <t>https://guardianlife.wd5.myworkdayjobs.com/Guardian-Life-Careers/job/New-York/Head-of-Cybersecurity-Assurance-Testing_R000108255</t>
+          <t>https://guardianlife.wd5.myworkdayjobs.com/Guardian-Life-Careers/job/Chennai/Senior-Engineer-IT_R000108657-1</t>
         </is>
       </c>
     </row>
@@ -1493,20 +1493,24 @@
       </c>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>Technical Product Owner/ Engineer</t>
+          <t>Lead, Cybersecurity Assurance Testing</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr">
         <is>
-          <t>Technical Product Owner/ Engineer Description The Technical Product Owner/ Engineer supports strategic modernization initiatives within the Financial Protection and Retirement Services Technology organization. The role partners closely with engineering teams to translate business needs into clear technical specifications, features, and system designs. This individual contributes hands‑on to technical discussions, solution design, and implementation support to ensure high‑quality delivery. This individual collaborates with product managers, business partners, and cross‑functional technical teams to shape technical solution. Strong knowledge of Agile is required to manage the backlog and drive iterative development. The individual will be deeply involved in hands-on technical activities such as development, supporting design decisions, creating technical requirements, and ensuring high‑quality implementation. You Are A self-starter, continuous learner and hands-on technical engineer who can translate vision from the Platform / Product D&amp;T leader into development by partnering across the engineers, product managers, business partners and executive stakeholders. You Will Lead the efforts of development team(s) consisting of resources spread across multiple time zones and countries. Work with offshore counterparts to coordinate completion of all team assignments, ensuring deadlines and milestones are met. Work with the development team(s) to ensure consistent software architecture and coding practices are used in all applications. Look for opportunities to create shared code modules to use across applications. Take a leadership and mentoring role when working with less experienced staff, always raising the bar of technical expertise within the organization. Inform project stakeholders on progress and potential problems that jeopardize deadlines and milestones. Make recommendations and modifications; remove obstacles. Help define roles and responsibilities within the development team. Be agile and flexible, shifting resources to align with changing priorities. As a Technical Product Owner/Engineer in a Product Operating Model: Partner closely with the Product Manager to shape and execute the product vision, roadmap, and prioritization based on customer and business value. Co-own backlog refinement by defining, writing, and prioritizing technical stories, spikes, and enablers; write clear Jira stories with acceptance criteria that reflect functional and technical needs. Align technical solutions with product strategy, long-term architecture, and non-functional requirements (security, performance, scalability, reliability). Drive an outcome-focused delivery approach using measurable objectives (e.g., OKRs) and product health metrics (e.g., reliability, cycle time, defect trends). Work with Business Product Owners and Agile Coaches on feasibility analysis, cost, and resource projections; facilitate architects and teams to generate technical design plans; ensure product specifications and quality standards are met. Operate across the full product lifecycle (build → release → run → improve): Collaborate with Production Support and Product teams to ensure seamless transition of features into production, maintain comprehensive documentation, and provide support for critical incidents as part of the product lifecycle. Establish and monitor product SLIs/SLOs, error budgets, and observability practices; use telemetry and customer feedback to inform prioritization and continuous improvement. Work with architects to determine the best technical solutions and applications for overall use in company products. Provide technical consultation to executive staff in determining competitive strategies. Lead implementation efforts for new applications and code updates. Work with enterprise and shared service teams on infrastructure setup, review board approvals, and deployment coordination. Stay abreast of new technology trends and advantages. Make recommendations for the direction of new and existing products. Define application roadmaps, including a strategy for minimizing technical debt and advancing modernization. Review and approve coding and documentation, user manuals, testing documentation, and procedures for existing and future applications. Ensure compliance with security, privacy, legal, infrastructure, and administrative/corporate processes and policies. Work with Production Support and other Shared Services teams in support of our products and customers. Salary Range: $99,150.00 - $162,885.00 The salary range reflected above is a good faith estimate of base pay for the primary location of the position. The salary for this position ultimately will be determined based on the education, experience, knowledge, and abilities of the successful candidate. In addition to salary, this role may also be eligible for annual, sales, or other incentive compensation. Our Promise At Guardian, you’ll have the support and flexibility to achieve your professional and personal goals.  Through skill-building, leadership development and philanthropic opportunities, we provide opportunities to build communities and grow your career, surrounded by diverse colleagues with high ethical standards. Inspire Well-Being As part of Guardian’s Purpose – to inspire well-being – we are committed to offering contemporary, supportive, flexible, and inclusive benefits and resources to our colleagues. Explore our company benefits at www.guardianlife.com/careers/corporate/benefits . Benefits apply to full-time eligible employees. Interns are not eligible for most Company benefits. Equal Employment Opportunity Guardian is an equal opportunity employer. All qualified applicants will be considered for employment without regard to age, race, color, creed, religion, sex, affectional or sexual orientation, national origin, ancestry, marital status, disability, military or veteran status, or any other classification protected by applicable law. Accommodations Guardian is committed to providing access, equal opportunity and reasonable accommodation for individuals with disabilities in employment, its services, programs, and activities. Guardian also provides reasonable accommodations to qualified job applicants (and employees) to accommodate the individual's known limitations related to pregnancy, childbirth, or related medical conditions, unless doing so would create an undue hardship. If reasonable accommodation is needed to participate in the job application or interview process, to perform essential job functions, and/or to receive other benefits and privileges of employment, please contact MyHR@glic.com. Please note: this resource is for accommodation requests only. For all other inquires related to your application and careers at Guardian, refer to the Guardian Careers site. Visa Sponsorship Guardian is not currently or in the foreseeable future sponsoring employment visas.  In order to be a successful applicant. you must be legally authorized to work in the United States, without the need for employer sponsorship. Current Guardian Colleagues: Please apply through the internal Jobs Hub in Workday.</t>
+          <t>Lead, Cyber Security Assurance Testing The Lead, Cyber Security Assurance Testing is a working‑lead / “player‑coach role” within Guardian’s Cybersecurity Assurance organization. This role includes formal people management responsibility for a small number of senior engineers, with a focus on operational and tactical planning ,execution, and reporting, contributing to strategic planning, and accountable for project and program outcomes. The role is structured roughly as: ~60% leadership, coordination, and program execution ~40% hands‑on technical contribution and research This position leads through influence, technical credibility, and ownership. It is designed for an experienced security professional who demonstrates ambition, strong execution discipline, and the potential to grow into broader leadership over time, while remaining close to the work today. The role supports and helps evolve Guardian’s Application Security Testing, Ethical Hacking (Red Team), and Third‑Party Testing programs, working closely with Cyber Defense, application owners, and Guardian India Security Assurance. Key Responsibilities Lead and coordinate day ‑ to ‑ day execution of: Application Security Testing Ethical Hacking / Red Team activities Third‑party penetration testing engagements Lead the Improvement and evolution of AppSec and Red Team programs, increasing consistency, structure, and measurable outcomes. Own and maintain processes, procedures, playbooks, and documentation to ensure clarity, repeatability, and quality. Contribute to and execute against program planning artifacts, including Roadmaps, backlogs, and quarterly and annual goals Coordinate work across US And India Based assurance staff and third party testing vendors. Remain actively involved in application security testing and ethical hacking, providing technical guidance and quality assurance Participate selectively in: Targeted application security testing Rating &amp; Validation of high‑risk or high‑impact findings Red‑team or adversarial exercises where appropriate Provide technical review and direction: Support security product evaluation, selection, proof‑of‑concepts, and implementation, ensuring tools are operationalized effectively. Communicate technical findings clearly and simply to non‑technical stakeholders. Translate testing results into risk‑based, actionable insights. Collaborate closely with Cyber Defense, application teams, and security stakeholders to ensure testing results lead to defensive improvements and remediation. Required Qualifications 5+ years of experience in application security testing, ethical hacking, or offensive security, with demonstrated leadership responsibility. Strong understanding of: Application security testing techniques Penetration testing vs. red team objectives Secure SDLC and risk-based testing Hands on technical experience validating vulnerabilities and testing application security controls. Experience improving or evolving existing security programs, rather than only building from scratch. Strong process orientation with proven ability to create practical, lightweight documentation. Excellent communication skills with the ability to explain technical concepts in simple, business relevant terms. Demonstrated ambition and intent to grow into broader leadership scope over time. Bachelor’s degree in a related field or equivalent experience/certifications. Preferred Qualifications Experience in financial services or other large, regulated enterprise environments. Exposure to cloud‑native application security and modern CI/CD environments. Experience working with globally distributed teams (e.g., US and India). Familiarity with AppSec and Offensive Security tools. Location Three days a week at our Guardian office in New York, NY or Bethlehem, PA Salary Range: $118,980.00 - $195,465.00 The salary range reflected above is a good faith estimate of base pay for the primary location of the position. The salary for this position ultimately will be determined based on the education, experience, knowledge, and abilities of the successful candidate. In addition to salary, this role may also be eligible for annual, sales, or other incentive compensation. Our Promise At Guardian, you’ll have the support and flexibility to achieve your professional and personal goals.  Through skill-building, leadership development and philanthropic opportunities, we provide opportunities to build communities and grow your career, surrounded by diverse colleagues with high ethical standards. Inspire Well-Being As part of Guardian’s Purpose – to inspire well-being – we are committed to offering contemporary, supportive, flexible, and inclusive benefits and resources to our colleagues. Explore our company benefits at www.guardianlife.com/careers/corporate/benefits . Benefits apply to full-time eligible employees. Interns are not eligible for most Company benefits. Equal Employment Opportunity Guardian is an equal opportunity employer. All qualified applicants will be considered for employment without regard to age, race, color, creed, religion, sex, affectional or sexual orientation, national origin, ancestry, marital status, disability, military or veteran status, or any other classification protected by applicable law. Accommodations Guardian is committed to providing access, equal opportunity and reasonable accommodation for individuals with disabilities in employment, its services, programs, and activities. Guardian also provides reasonable accommodations to qualified job applicants (and employees) to accommodate the individual's known limitations related to pregnancy, childbirth, or related medical conditions, unless doing so would create an undue hardship. If reasonable accommodation is needed to participate in the job application or interview process, to perform essential job functions, and/or to receive other benefits and privileges of employment, please contact MyHR@glic.com. Please note: this resource is for accommodation requests only. For all other inquires related to your application and careers at Guardian, refer to the Guardian Careers site. Visa Sponsorship Guardian is not currently or in the foreseeable future sponsoring employment visas.  In order to be a successful applicant. you must be legally authorized to work in the United States, without the need for employer sponsorship. Current Guardian Colleagues: Please apply through the internal Jobs Hub in Workday.</t>
         </is>
       </c>
       <c r="D24" s="3" t="inlineStr">
         <is>
-          <t>Holmdel</t>
-        </is>
-      </c>
-      <c r="E24" s="3" t="inlineStr"/>
+          <t>New York</t>
+        </is>
+      </c>
+      <c r="E24" s="3" t="inlineStr">
+        <is>
+          <t>Bethlehem</t>
+        </is>
+      </c>
       <c r="F24" s="3" t="inlineStr">
         <is>
           <t>2026-02-13</t>
@@ -1514,7 +1518,7 @@
       </c>
       <c r="G24" s="3" t="inlineStr">
         <is>
-          <t>R000108473</t>
+          <t>R000108255</t>
         </is>
       </c>
       <c r="H24" s="3" t="inlineStr">
@@ -1524,7 +1528,7 @@
       </c>
       <c r="I24" s="3" t="inlineStr">
         <is>
-          <t>https://guardianlife.wd5.myworkdayjobs.com/Guardian-Life-Careers/job/Holmdel/Technical-Product-Owner--Engineer_R000108473</t>
+          <t>https://guardianlife.wd5.myworkdayjobs.com/Guardian-Life-Careers/job/New-York/Head-of-Cybersecurity-Assurance-Testing_R000108255</t>
         </is>
       </c>
     </row>
@@ -1536,24 +1540,20 @@
       </c>
       <c r="B25" s="4" t="inlineStr">
         <is>
-          <t>Actuarial Product Consultant</t>
+          <t>Technical Product Owner/ Engineer</t>
         </is>
       </c>
       <c r="C25" s="4" t="inlineStr">
         <is>
-          <t>Is the opportunity to join a culture where “We Do the Right Thing,” and “We Courageously Shape Our Future Together” important to you? If so, Guardian is seeking a resolute motivated individual to join our team as an Actuarial Product Consultant. This role will be part of Guardian’s Annuity Pricing and Structured Solutions Team. The successful candidate will play a crucial and multifaceted role in the context of pricing, development, and support of existing and new annuity products. This position requires a curious, technically proficient, and highly analytical individual who enjoys sophisticated solutions design including hands-on modeling and contributing to regular as well as exploratory product pricing. This is a visible role that involves collaboration with multiple areas, including product development, valuation, finance, hedging, reinsurance, IT, legal, and corporate actuarial. You are An actuary with a passion for both ALM modeling and economic analysis/risk management and with the ability to communicate effectively to a wider audience. You are skilled at applying actuarial principles, logic, programming, and business knowledge to solve complex problems. You will Collaborate with cross-functional teams to support pricing strategy and NBV reporting for existing and future annuity products. Conduct detailed actuarial analysis and modeling to ensure accuracy in pricing and reporting. Assist in the development and validation of actuarial models, ensuring compliance with company and regulatory model governance standards. Lead or contribute to projects related to new product development and enhancements to existing annuity models and offerings. Work closely with senior leadership to align pricing strategies with overall business objectives. Perform ad hoc analysis and provide actuarial support to cross-functional teams. Communicate the results to senior leaders through well-organized and documented spreadsheets, PowerPoint presentations, memos, and emails. You have Recent FSA designation from the Society of Actuaries required. 5+ years of Insurance relevant experience preferably in areas such as product pricing, Economic Capital or Cash Flow Testing modeling and reporting. Experience with asset and/or liability modeling in GGY AXIS required. Knowledge of financial derivatives and hedging is a plus. Experience with Python and VBA is a plus. Excellent analytical, problem-solving, and communication skills. Knowledge of individual or group annuity products, such as Income annuity, MYGA, Registered Index Linked Annuities and Fixed Index Annuities or group in-plan annuity solutions is a plus. Ability to work independently and lead multiple projects in a collaborative team environment. Proficiency in Microsoft Office. Reporting Relationships: T his role reports to the Head of Annuity Pricing, who reports to the Head of Annuities . Location: Hybrid role - 3 days in a Guardian office located in Hudson Yards, NYC or Holmdel, NJ. 2 days WFH. Salary Range: $152,290.00 - $250,195.00 The salary range reflected above is a good faith estimate of base pay for the primary location of the position. The salary for this position ultimately will be determined based on the education, experience, knowledge, and abilities of the successful candidate. In addition to salary, this role may also be eligible for annual, sales, or other incentive compensation. Our Promise At Guardian, you’ll have the support and flexibility to achieve your professional and personal goals.  Through skill-building, leadership development and philanthropic opportunities, we provide opportunities to build communities and grow your career, surrounded by diverse colleagues with high ethical standards. Inspire Well-Being As part of Guardian’s Purpose – to inspire well-being – we are committed to offering contemporary, supportive, flexible, and inclusive benefits and resources to our colleagues. Explore our company benefits at www.guardianlife.com/careers/corporate/benefits . Benefits apply to full-time eligible employees. Interns are not eligible for most Company benefits. Equal Employment Opportunity Guardian is an equal opportunity employer. All qualified applicants will be considered for employment without regard to age, race, color, creed, religion, sex, affectional or sexual orientation, national origin, ancestry, marital status, disability, military or veteran status, or any other classification protected by applicable law. Accommodations Guardian is committed to providing access, equal opportunity and reasonable accommodation for individuals with disabilities in employment, its services, programs, and activities. Guardian also provides reasonable accommodations to qualified job applicants (and employees) to accommodate the individual's known limitations related to pregnancy, childbirth, or related medical conditions, unless doing so would create an undue hardship. If reasonable accommodation is needed to participate in the job application or interview process, to perform essential job functions, and/or to receive other benefits and privileges of employment, please contact MyHR@glic.com. Please note: this resource is for accommodation requests only. For all other inquires related to your application and careers at Guardian, refer to the Guardian Careers site. Visa Sponsorship Guardian is not currently or in the foreseeable future sponsoring employment visas.  In order to be a successful applicant. you must be legally authorized to work in the United States, without the need for employer sponsorship. Current Guardian Colleagues: Please apply through the internal Jobs Hub in Workday.</t>
+          <t>Technical Product Owner/ Engineer Description The Technical Product Owner/ Engineer supports strategic modernization initiatives within the Financial Protection and Retirement Services Technology organization. The role partners closely with engineering teams to translate business needs into clear technical specifications, features, and system designs. This individual contributes hands‑on to technical discussions, solution design, and implementation support to ensure high‑quality delivery. This individual collaborates with product managers, business partners, and cross‑functional technical teams to shape technical solution. Strong knowledge of Agile is required to manage the backlog and drive iterative development. The individual will be deeply involved in hands-on technical activities such as development, supporting design decisions, creating technical requirements, and ensuring high‑quality implementation. You Are A self-starter, continuous learner and hands-on technical engineer who can translate vision from the Platform / Product D&amp;T leader into development by partnering across the engineers, product managers, business partners and executive stakeholders. You Will Lead the efforts of development team(s) consisting of resources spread across multiple time zones and countries. Work with offshore counterparts to coordinate completion of all team assignments, ensuring deadlines and milestones are met. Work with the development team(s) to ensure consistent software architecture and coding practices are used in all applications. Look for opportunities to create shared code modules to use across applications. Take a leadership and mentoring role when working with less experienced staff, always raising the bar of technical expertise within the organization. Inform project stakeholders on progress and potential problems that jeopardize deadlines and milestones. Make recommendations and modifications; remove obstacles. Help define roles and responsibilities within the development team. Be agile and flexible, shifting resources to align with changing priorities. As a Technical Product Owner/Engineer in a Product Operating Model: Partner closely with the Product Manager to shape and execute the product vision, roadmap, and prioritization based on customer and business value. Co-own backlog refinement by defining, writing, and prioritizing technical stories, spikes, and enablers; write clear Jira stories with acceptance criteria that reflect functional and technical needs. Align technical solutions with product strategy, long-term architecture, and non-functional requirements (security, performance, scalability, reliability). Drive an outcome-focused delivery approach using measurable objectives (e.g., OKRs) and product health metrics (e.g., reliability, cycle time, defect trends). Work with Business Product Owners and Agile Coaches on feasibility analysis, cost, and resource projections; facilitate architects and teams to generate technical design plans; ensure product specifications and quality standards are met. Operate across the full product lifecycle (build → release → run → improve): Collaborate with Production Support and Product teams to ensure seamless transition of features into production, maintain comprehensive documentation, and provide support for critical incidents as part of the product lifecycle. Establish and monitor product SLIs/SLOs, error budgets, and observability practices; use telemetry and customer feedback to inform prioritization and continuous improvement. Work with architects to determine the best technical solutions and applications for overall use in company products. Provide technical consultation to executive staff in determining competitive strategies. Lead implementation efforts for new applications and code updates. Work with enterprise and shared service teams on infrastructure setup, review board approvals, and deployment coordination. Stay abreast of new technology trends and advantages. Make recommendations for the direction of new and existing products. Define application roadmaps, including a strategy for minimizing technical debt and advancing modernization. Review and approve coding and documentation, user manuals, testing documentation, and procedures for existing and future applications. Ensure compliance with security, privacy, legal, infrastructure, and administrative/corporate processes and policies. Work with Production Support and other Shared Services teams in support of our products and customers. Salary Range: $99,150.00 - $162,885.00 The salary range reflected above is a good faith estimate of base pay for the primary location of the position. The salary for this position ultimately will be determined based on the education, experience, knowledge, and abilities of the successful candidate. In addition to salary, this role may also be eligible for annual, sales, or other incentive compensation. Our Promise At Guardian, you’ll have the support and flexibility to achieve your professional and personal goals.  Through skill-building, leadership development and philanthropic opportunities, we provide opportunities to build communities and grow your career, surrounded by diverse colleagues with high ethical standards. Inspire Well-Being As part of Guardian’s Purpose – to inspire well-being – we are committed to offering contemporary, supportive, flexible, and inclusive benefits and resources to our colleagues. Explore our company benefits at www.guardianlife.com/careers/corporate/benefits . Benefits apply to full-time eligible employees. Interns are not eligible for most Company benefits. Equal Employment Opportunity Guardian is an equal opportunity employer. All qualified applicants will be considered for employment without regard to age, race, color, creed, religion, sex, affectional or sexual orientation, national origin, ancestry, marital status, disability, military or veteran status, or any other classification protected by applicable law. Accommodations Guardian is committed to providing access, equal opportunity and reasonable accommodation for individuals with disabilities in employment, its services, programs, and activities. Guardian also provides reasonable accommodations to qualified job applicants (and employees) to accommodate the individual's known limitations related to pregnancy, childbirth, or related medical conditions, unless doing so would create an undue hardship. If reasonable accommodation is needed to participate in the job application or interview process, to perform essential job functions, and/or to receive other benefits and privileges of employment, please contact MyHR@glic.com. Please note: this resource is for accommodation requests only. For all other inquires related to your application and careers at Guardian, refer to the Guardian Careers site. Visa Sponsorship Guardian is not currently or in the foreseeable future sponsoring employment visas.  In order to be a successful applicant. you must be legally authorized to work in the United States, without the need for employer sponsorship. Current Guardian Colleagues: Please apply through the internal Jobs Hub in Workday.</t>
         </is>
       </c>
       <c r="D25" s="4" t="inlineStr">
         <is>
-          <t>New York</t>
-        </is>
-      </c>
-      <c r="E25" s="4" t="inlineStr">
-        <is>
           <t>Holmdel</t>
         </is>
       </c>
+      <c r="E25" s="4" t="inlineStr"/>
       <c r="F25" s="4" t="inlineStr">
         <is>
           <t>2026-02-13</t>
@@ -1561,7 +1561,7 @@
       </c>
       <c r="G25" s="4" t="inlineStr">
         <is>
-          <t>R000108508</t>
+          <t>R000108473</t>
         </is>
       </c>
       <c r="H25" s="4" t="inlineStr">
@@ -1571,7 +1571,7 @@
       </c>
       <c r="I25" s="4" t="inlineStr">
         <is>
-          <t>https://guardianlife.wd5.myworkdayjobs.com/Guardian-Life-Careers/job/New-York/Actuarial-Product-Consultant_R000108508</t>
+          <t>https://guardianlife.wd5.myworkdayjobs.com/Guardian-Life-Careers/job/Holmdel/Technical-Product-Owner--Engineer_R000108473</t>
         </is>
       </c>
     </row>
@@ -1583,38 +1583,42 @@
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>DI Medical Underwriting Consultant</t>
+          <t>Actuarial Product Consultant</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr">
         <is>
-          <t>The DI Underwriting Medical Consultant , reporting to the Manager, Underwriting Policy and Support in the Underwriting Policy area, is a key business partner for DI Underwriting. This position assists in maintaining the DI underwriting guidelines and is responsible for reviewing individual health risk characteristics for complicated applicants, assisting in making recommendations to underwriting. The role combines clinical judgment, analytics, and strong communication. The applicant should be a medical professional who can understand health conditions and personal characteristics, singly and in combination, and how they influence the probability of disability. You will Assist with medical reviews of current underwriting cases Review older underwriting and claims files when needed to support ongoing IDI underwriting policy research projects Medical guideline authorship, drafting, updating and driving change across underwriting Review medical literature to remain up to date on current medical best practices Assist in keeping the underwriting guidelines current and relevant Collaborate cross functionally with underwriting leadership, claims, legal/compliance, data, etc. You have Bachelor of Science in Nursing (BSN) degree required 5+ years of clinical experience in high-acuity settings cardiac care, ER/ICU, or case management experience Strong ability to interpret common cardiac testing; including EKG’s Solid proficiency with Microsoft 365 (Word, Excel, PowerPoint) Business mindset, familiarity with statistics, prior insurance or disability experience a plus Skills and Competencies: Clinical Synthesis for IDI: Training and experience with many varied medical conditions is essential.  This includes recognition of symptoms, knowledge of medications that are commonly used to treat various ailments, ability to understand and interpret medical records, and an understanding of treatments and durations of a wide range of diseases. Risk Decisioning: Clear understanding of risk management is central to this position.  Morbidity risk is the driving force of profitability in this profit center.  The person in this role must understand when to offer a policy to an applicant with a less-than-ideal medical history, when to modify the benefits of the policy prior to issue, and when to decline the policy altogether. Communication: This skill is vital, since the person in this position must answer medical questions from underwriters daily, and the answers must be clear and actionable. Operations Prioritization: The medical underwriting queue has turned around times that must be managed efficiently with additional job roles. Collaboration and Professionalism: Individual will be an effective partner to Underwriting, Claims, and Legal/Compliance. LOCATION This is a remote position. Salary Range: $73,280.00 - $120,395.00 The salary range reflected above is a good faith estimate of base pay for the primary location of the position. The salary for this position ultimately will be determined based on the education, experience, knowledge, and abilities of the successful candidate. In addition to salary, this role may also be eligible for annual, sales, or other incentive compensation. Our Promise At Guardian, you’ll have the support and flexibility to achieve your professional and personal goals.  Through skill-building, leadership development and philanthropic opportunities, we provide opportunities to build communities and grow your career, surrounded by diverse colleagues with high ethical standards. Inspire Well-Being As part of Guardian’s Purpose – to inspire well-being – we are committed to offering contemporary, supportive, flexible, and inclusive benefits and resources to our colleagues. Explore our company benefits at www.guardianlife.com/careers/corporate/benefits . Benefits apply to full-time eligible employees. Interns are not eligible for most Company benefits. Equal Employment Opportunity Guardian is an equal opportunity employer. All qualified applicants will be considered for employment without regard to age, race, color, creed, religion, sex, affectional or sexual orientation, national origin, ancestry, marital status, disability, military or veteran status, or any other classification protected by applicable law. Accommodations Guardian is committed to providing access, equal opportunity and reasonable accommodation for individuals with disabilities in employment, its services, programs, and activities. Guardian also provides reasonable accommodations to qualified job applicants (and employees) to accommodate the individual's known limitations related to pregnancy, childbirth, or related medical conditions, unless doing so would create an undue hardship. If reasonable accommodation is needed to participate in the job application or interview process, to perform essential job functions, and/or to receive other benefits and privileges of employment, please contact MyHR@glic.com. Please note: this resource is for accommodation requests only. For all other inquires related to your application and careers at Guardian, refer to the Guardian Careers site. Visa Sponsorship Guardian is not currently or in the foreseeable future sponsoring employment visas.  In order to be a successful applicant. you must be legally authorized to work in the United States, without the need for employer sponsorship. Current Guardian Colleagues: Please apply through the internal Jobs Hub in Workday.</t>
+          <t>Is the opportunity to join a culture where “We Do the Right Thing,” and “We Courageously Shape Our Future Together” important to you? If so, Guardian is seeking a resolute motivated individual to join our team as an Actuarial Product Consultant. This role will be part of Guardian’s Annuity Pricing and Structured Solutions Team. The successful candidate will play a crucial and multifaceted role in the context of pricing, development, and support of existing and new annuity products. This position requires a curious, technically proficient, and highly analytical individual who enjoys sophisticated solutions design including hands-on modeling and contributing to regular as well as exploratory product pricing. This is a visible role that involves collaboration with multiple areas, including product development, valuation, finance, hedging, reinsurance, IT, legal, and corporate actuarial. You are An actuary with a passion for both ALM modeling and economic analysis/risk management and with the ability to communicate effectively to a wider audience. You are skilled at applying actuarial principles, logic, programming, and business knowledge to solve complex problems. You will Collaborate with cross-functional teams to support pricing strategy and NBV reporting for existing and future annuity products. Conduct detailed actuarial analysis and modeling to ensure accuracy in pricing and reporting. Assist in the development and validation of actuarial models, ensuring compliance with company and regulatory model governance standards. Lead or contribute to projects related to new product development and enhancements to existing annuity models and offerings. Work closely with senior leadership to align pricing strategies with overall business objectives. Perform ad hoc analysis and provide actuarial support to cross-functional teams. Communicate the results to senior leaders through well-organized and documented spreadsheets, PowerPoint presentations, memos, and emails. You have Recent FSA designation from the Society of Actuaries required. 5+ years of Insurance relevant experience preferably in areas such as product pricing, Economic Capital or Cash Flow Testing modeling and reporting. Experience with asset and/or liability modeling in GGY AXIS required. Knowledge of financial derivatives and hedging is a plus. Experience with Python and VBA is a plus. Excellent analytical, problem-solving, and communication skills. Knowledge of individual or group annuity products, such as Income annuity, MYGA, Registered Index Linked Annuities and Fixed Index Annuities or group in-plan annuity solutions is a plus. Ability to work independently and lead multiple projects in a collaborative team environment. Proficiency in Microsoft Office. Reporting Relationships: T his role reports to the Head of Annuity Pricing, who reports to the Head of Annuities . Location: Hybrid role - 3 days in a Guardian office located in Hudson Yards, NYC or Holmdel, NJ. 2 days WFH. Salary Range: $152,290.00 - $250,195.00 The salary range reflected above is a good faith estimate of base pay for the primary location of the position. The salary for this position ultimately will be determined based on the education, experience, knowledge, and abilities of the successful candidate. In addition to salary, this role may also be eligible for annual, sales, or other incentive compensation. Our Promise At Guardian, you’ll have the support and flexibility to achieve your professional and personal goals.  Through skill-building, leadership development and philanthropic opportunities, we provide opportunities to build communities and grow your career, surrounded by diverse colleagues with high ethical standards. Inspire Well-Being As part of Guardian’s Purpose – to inspire well-being – we are committed to offering contemporary, supportive, flexible, and inclusive benefits and resources to our colleagues. Explore our company benefits at www.guardianlife.com/careers/corporate/benefits . Benefits apply to full-time eligible employees. Interns are not eligible for most Company benefits. Equal Employment Opportunity Guardian is an equal opportunity employer. All qualified applicants will be considered for employment without regard to age, race, color, creed, religion, sex, affectional or sexual orientation, national origin, ancestry, marital status, disability, military or veteran status, or any other classification protected by applicable law. Accommodations Guardian is committed to providing access, equal opportunity and reasonable accommodation for individuals with disabilities in employment, its services, programs, and activities. Guardian also provides reasonable accommodations to qualified job applicants (and employees) to accommodate the individual's known limitations related to pregnancy, childbirth, or related medical conditions, unless doing so would create an undue hardship. If reasonable accommodation is needed to participate in the job application or interview process, to perform essential job functions, and/or to receive other benefits and privileges of employment, please contact MyHR@glic.com. Please note: this resource is for accommodation requests only. For all other inquires related to your application and careers at Guardian, refer to the Guardian Careers site. Visa Sponsorship Guardian is not currently or in the foreseeable future sponsoring employment visas.  In order to be a successful applicant. you must be legally authorized to work in the United States, without the need for employer sponsorship. Current Guardian Colleagues: Please apply through the internal Jobs Hub in Workday.</t>
         </is>
       </c>
       <c r="D26" s="3" t="inlineStr">
         <is>
-          <t>Remote - United States</t>
-        </is>
-      </c>
-      <c r="E26" s="3" t="inlineStr"/>
+          <t>New York</t>
+        </is>
+      </c>
+      <c r="E26" s="3" t="inlineStr">
+        <is>
+          <t>Holmdel</t>
+        </is>
+      </c>
       <c r="F26" s="3" t="inlineStr">
         <is>
-          <t>2026-02-12</t>
+          <t>2026-02-13</t>
         </is>
       </c>
       <c r="G26" s="3" t="inlineStr">
         <is>
-          <t>R000108610</t>
+          <t>R000108508</t>
         </is>
       </c>
       <c r="H26" s="3" t="inlineStr">
         <is>
-          <t>Fully Remote</t>
+          <t>Hybrid - In office 3 days per week</t>
         </is>
       </c>
       <c r="I26" s="3" t="inlineStr">
         <is>
-          <t>https://guardianlife.wd5.myworkdayjobs.com/Guardian-Life-Careers/job/Remote---United-States/DI-Medical-Underwriting-Consultant_R000108610</t>
+          <t>https://guardianlife.wd5.myworkdayjobs.com/Guardian-Life-Careers/job/New-York/Actuarial-Product-Consultant_R000108508</t>
         </is>
       </c>
     </row>
@@ -1626,24 +1630,20 @@
       </c>
       <c r="B27" s="4" t="inlineStr">
         <is>
-          <t>PEO and Aggregator Strategy &amp; Operations Lead</t>
+          <t>DI Medical Underwriting Consultant</t>
         </is>
       </c>
       <c r="C27" s="4" t="inlineStr">
         <is>
-          <t>PEO and Aggregator Strategy &amp; Operations Lead role, will be accountable for providing thought leadership capabilities, and tools to maximize the growth potential of one of our fastest growing Distribution segments. The primary focus will be with PEO’s and technology aggregators that operate in the non-traditional group insurance space. You will partner with various functional partners and stakeholders to deliver operational excellence for Guardian partners and clients while always leading with a customer mindset. Ultimately, you provide the ongoing capabilities necessary to drive market-leading differentiation through specialized solutions that anticipate the evolving needs of our distribution partners and clients and meet Guardian’s objective of driving sustainable industry leading profitable revenue growth. You will report directly to the Head of Distribution Strategy and Market Management within Group Benefits You Will: Be accountable for driving operational and system enhancements that create a differentiated customer experience within one of our fastest growing distribution channels Partner with the field to identify channel partner needs, drive alignment and and manage portfolio of capability investments Engage with functional stakeholders to ensure resource capacity and strategic alignment to meet channel needs Support effective distribution execution by providing the right tools/processes and building the right knowledge Serve as SME for operational processes and best practices serving the needs of Key Markets partners Act as the business owner for bringing new opportunities to market Articulate channel needs and influence support across organizational initiatives to ensure channel needs are met for new capabilities and solutions Partner with client management to expand upon solutions leveraged in market to drive employer and member engagement in benefits Facilitate the need for expanded technical and integration capabilities Engage on high profile partner initiatives as needed You Have: Minimum of 8 years in distribution facing operations roles for a multi-faceted corporation (insurance industry preferred). Deep expertise in specialty and alternative distribution models and associated operational needs. Proven success in designing and implementing innovative strategies to enhance the customer experience in a digital consumer-centric ecosystem. A strong process and system orientation and an ability to identify impacts of change while optimizing business value. Strong general management mindset and experience with broad functional strategy development and execution. Commercial insurance, financial services and/or management consulting experience preferred. Strong background in business case development and execution. High energy with strong executive presence and public speaking skills including presentation to C-Suite, as well as field stakeholders. Relentless focus on innovative strategic thought leadership and a track record of success in affecting change, having delivered quantifiable impact on company revenue. Compelling presentation skills e.g. comfortable speaking at large group conferences and webinars. Location, Work Arrangement, and Travel: Preferred locations for this position include New York, NY; Holmdel, NJ; Boston, MA; and Bethlehem, PA. The work arrangement will be hybrid (three days per week in a local Guardian Office; two days working from home). Approximately 10-15% travel associated with this position. Salary Range: $118,980.00 - $195,465.00 The salary range reflected above is a good faith estimate of base pay for the primary location of the position. The salary for this position ultimately will be determined based on the education, experience, knowledge, and abilities of the successful candidate. In addition to salary, this role may also be eligible for annual, sales, or other incentive compensation. Our Promise At Guardian, you’ll have the support and flexibility to achieve your professional and personal goals.  Through skill-building, leadership development and philanthropic opportunities, we provide opportunities to build communities and grow your career, surrounded by diverse colleagues with high ethical standards. Inspire Well-Being As part of Guardian’s Purpose – to inspire well-being – we are committed to offering contemporary, supportive, flexible, and inclusive benefits and resources to our colleagues. Explore our company benefits at www.guardianlife.com/careers/corporate/benefits . Benefits apply to full-time eligible employees. Interns are not eligible for most Company benefits. Equal Employment Opportunity Guardian is an equal opportunity employer. All qualified applicants will be considered for employment without regard to age, race, color, creed, religion, sex, affectional or sexual orientation, national origin, ancestry, marital status, disability, military or veteran status, or any other classification protected by applicable law. Accommodations Guardian is committed to providing access, equal opportunity and reasonable accommodation for individuals with disabilities in employment, its services, programs, and activities. Guardian also provides reasonable accommodations to qualified job applicants (and employees) to accommodate the individual's known limitations related to pregnancy, childbirth, or related medical conditions, unless doing so would create an undue hardship. If reasonable accommodation is needed to participate in the job application or interview process, to perform essential job functions, and/or to receive other benefits and privileges of employment, please contact MyHR@glic.com. Please note: this resource is for accommodation requests only. For all other inquires related to your application and careers at Guardian, refer to the Guardian Careers site. Visa Sponsorship Guardian is not currently or in the foreseeable future sponsoring employment visas.  In order to be a successful applicant. you must be legally authorized to work in the United States, without the need for employer sponsorship. Current Guardian Colleagues: Please apply through the internal Jobs Hub in Workday.</t>
+          <t>The DI Underwriting Medical Consultant , reporting to the Manager, Underwriting Policy and Support in the Underwriting Policy area, is a key business partner for DI Underwriting. This position assists in maintaining the DI underwriting guidelines and is responsible for reviewing individual health risk characteristics for complicated applicants, assisting in making recommendations to underwriting. The role combines clinical judgment, analytics, and strong communication. The applicant should be a medical professional who can understand health conditions and personal characteristics, singly and in combination, and how they influence the probability of disability. You will Assist with medical reviews of current underwriting cases Review older underwriting and claims files when needed to support ongoing IDI underwriting policy research projects Medical guideline authorship, drafting, updating and driving change across underwriting Review medical literature to remain up to date on current medical best practices Assist in keeping the underwriting guidelines current and relevant Collaborate cross functionally with underwriting leadership, claims, legal/compliance, data, etc. You have Bachelor of Science in Nursing (BSN) degree required 5+ years of clinical experience in high-acuity settings cardiac care, ER/ICU, or case management experience Strong ability to interpret common cardiac testing; including EKG’s Solid proficiency with Microsoft 365 (Word, Excel, PowerPoint) Business mindset, familiarity with statistics, prior insurance or disability experience a plus Skills and Competencies: Clinical Synthesis for IDI: Training and experience with many varied medical conditions is essential.  This includes recognition of symptoms, knowledge of medications that are commonly used to treat various ailments, ability to understand and interpret medical records, and an understanding of treatments and durations of a wide range of diseases. Risk Decisioning: Clear understanding of risk management is central to this position.  Morbidity risk is the driving force of profitability in this profit center.  The person in this role must understand when to offer a policy to an applicant with a less-than-ideal medical history, when to modify the benefits of the policy prior to issue, and when to decline the policy altogether. Communication: This skill is vital, since the person in this position must answer medical questions from underwriters daily, and the answers must be clear and actionable. Operations Prioritization: The medical underwriting queue has turned around times that must be managed efficiently with additional job roles. Collaboration and Professionalism: Individual will be an effective partner to Underwriting, Claims, and Legal/Compliance. LOCATION This is a remote position. Salary Range: $73,280.00 - $120,395.00 The salary range reflected above is a good faith estimate of base pay for the primary location of the position. The salary for this position ultimately will be determined based on the education, experience, knowledge, and abilities of the successful candidate. In addition to salary, this role may also be eligible for annual, sales, or other incentive compensation. Our Promise At Guardian, you’ll have the support and flexibility to achieve your professional and personal goals.  Through skill-building, leadership development and philanthropic opportunities, we provide opportunities to build communities and grow your career, surrounded by diverse colleagues with high ethical standards. Inspire Well-Being As part of Guardian’s Purpose – to inspire well-being – we are committed to offering contemporary, supportive, flexible, and inclusive benefits and resources to our colleagues. Explore our company benefits at www.guardianlife.com/careers/corporate/benefits . Benefits apply to full-time eligible employees. Interns are not eligible for most Company benefits. Equal Employment Opportunity Guardian is an equal opportunity employer. All qualified applicants will be considered for employment without regard to age, race, color, creed, religion, sex, affectional or sexual orientation, national origin, ancestry, marital status, disability, military or veteran status, or any other classification protected by applicable law. Accommodations Guardian is committed to providing access, equal opportunity and reasonable accommodation for individuals with disabilities in employment, its services, programs, and activities. Guardian also provides reasonable accommodations to qualified job applicants (and employees) to accommodate the individual's known limitations related to pregnancy, childbirth, or related medical conditions, unless doing so would create an undue hardship. If reasonable accommodation is needed to participate in the job application or interview process, to perform essential job functions, and/or to receive other benefits and privileges of employment, please contact MyHR@glic.com. Please note: this resource is for accommodation requests only. For all other inquires related to your application and careers at Guardian, refer to the Guardian Careers site. Visa Sponsorship Guardian is not currently or in the foreseeable future sponsoring employment visas.  In order to be a successful applicant. you must be legally authorized to work in the United States, without the need for employer sponsorship. Current Guardian Colleagues: Please apply through the internal Jobs Hub in Workday.</t>
         </is>
       </c>
       <c r="D27" s="4" t="inlineStr">
         <is>
-          <t>New York</t>
-        </is>
-      </c>
-      <c r="E27" s="4" t="inlineStr">
-        <is>
-          <t>Bethlehem, Boston, Holmdel</t>
-        </is>
-      </c>
+          <t>Remote - United States</t>
+        </is>
+      </c>
+      <c r="E27" s="4" t="inlineStr"/>
       <c r="F27" s="4" t="inlineStr">
         <is>
           <t>2026-02-12</t>
@@ -1651,17 +1651,17 @@
       </c>
       <c r="G27" s="4" t="inlineStr">
         <is>
-          <t>R000108155</t>
+          <t>R000108610</t>
         </is>
       </c>
       <c r="H27" s="4" t="inlineStr">
         <is>
-          <t>Hybrid - In office 3 days per week</t>
+          <t>Fully Remote</t>
         </is>
       </c>
       <c r="I27" s="4" t="inlineStr">
         <is>
-          <t>https://guardianlife.wd5.myworkdayjobs.com/Guardian-Life-Careers/job/New-York/Key-Markets-Strategy---Operations-Lead--Group-Benefits_R000108155</t>
+          <t>https://guardianlife.wd5.myworkdayjobs.com/Guardian-Life-Careers/job/Remote---United-States/DI-Medical-Underwriting-Consultant_R000108610</t>
         </is>
       </c>
     </row>
@@ -1673,20 +1673,24 @@
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>Associate Sales Representative, Group Benefits</t>
+          <t>PEO and Aggregator Strategy &amp; Operations Lead</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
         <is>
-          <t>Guardian's Group Benefits team is seeking Associate Sales Representative who will be responsible for building and maintaining brokers and plan holder relationships to drive ongoing sales and retention of groups of 2-2,000 lives with a primary focus on the under 100 lives market. Success will be determined based on the ability to attain high levels of production through broker development and internal relationships. This role will report to the Market Leader within the assigned territory. You Will: Market, position, and sell Guardian’s entire Group Benefits portfolio products and technology solutions to your designated brokers. This includes Dental, Vision, Life, Disability, Absence, and Supplemental Health products. Support the general wellbeing of the broker and client relationship for the development and growth of Guardian sales and client retention. Understand territory dynamics to build, develop and maintain broker relationships to grow the book of business while representing Guardian’s vision to inspire well-being. Be accountable for consistently achieving or exceeding personal sales production expectations by having a clear understanding of products. Identify, recommend and champion process improvements and organizational initiatives to increase sales of product offerings. Achieve required industry licensing within 90 days of date of hire and maintain license through completing Continuing Education requirements. You Have: A BA/BS degree or equivalent work experience Ability to consistently achieve or exceed personal sales production expectations established by management, as stated in the Market business plan that is consistent with Group Profit Center objectives. Soft Skills: Collaborative team player with the ability to effectively build rapport in person and virtually. Exercise sound judgement and integrity in a changing, matrixed, and fast past environment. Exude confidence, positivity, and proactivity. Act with accountability to deliver on commitments with speed and quality. Location and Travel Requirements: Successful hire must be based in the Atlanta, GA area Up to 20% travel within the U.S. Salary: $35,000 ​ The salary reflected above is a good faith estimate of base pay for the primary location of the position. The salary for this position ultimately will be determined based on the education, experience, knowledge, and abilities of the successful candidate. In addition to salary, this role may also be eligible for annual, sales, or other incentive compensation. Our Promise At Guardian, you’ll have the support and flexibility to achieve your professional and personal goals.  Through skill-building, leadership development and philanthropic opportunities, we provide opportunities to build communities and grow your career, surrounded by diverse colleagues with high ethical standards. Inspire Well-Being As part of Guardian’s Purpose – to inspire well-being – we are committed to offering contemporary, supportive, flexible, and inclusive benefits and resources to our colleagues. Explore our company benefits at www.guardianlife.com/careers/corporate/benefits . Benefits apply to full-time eligible employees. Interns are not eligible for most Company benefits. Equal Employment Opportunity Guardian is an equal opportunity employer. All qualified applicants will be considered for employment without regard to age, race, color, creed, religion, sex, affectional or sexual orientation, national origin, ancestry, marital status, disability, military or veteran status, or any other classification protected by applicable law. Accommodations Guardian is committed to providing access, equal opportunity and reasonable accommodation for individuals with disabilities in employment, its services, programs, and activities. Guardian also provides reasonable accommodations to qualified job applicants (and employees) to accommodate the individual's known limitations related to pregnancy, childbirth, or related medical conditions, unless doing so would create an undue hardship. If reasonable accommodation is needed to participate in the job application or interview process, to perform essential job functions, and/or to receive other benefits and privileges of employment, please contact MyHR@glic.com. Please note: this resource is for accommodation requests only. For all other inquires related to your application and careers at Guardian, refer to the Guardian Careers site. Visa Sponsorship Guardian is not currently or in the foreseeable future sponsoring employment visas.  In order to be a successful applicant. you must be legally authorized to work in the United States, without the need for employer sponsorship. Current Guardian Colleagues: Please apply through the internal Jobs Hub in Workday</t>
+          <t>PEO and Aggregator Strategy &amp; Operations Lead role, will be accountable for providing thought leadership capabilities, and tools to maximize the growth potential of one of our fastest growing Distribution segments. The primary focus will be with PEO’s and technology aggregators that operate in the non-traditional group insurance space. You will partner with various functional partners and stakeholders to deliver operational excellence for Guardian partners and clients while always leading with a customer mindset. Ultimately, you provide the ongoing capabilities necessary to drive market-leading differentiation through specialized solutions that anticipate the evolving needs of our distribution partners and clients and meet Guardian’s objective of driving sustainable industry leading profitable revenue growth. You will report directly to the Head of Distribution Strategy and Market Management within Group Benefits You Will: Be accountable for driving operational and system enhancements that create a differentiated customer experience within one of our fastest growing distribution channels Partner with the field to identify channel partner needs, drive alignment and and manage portfolio of capability investments Engage with functional stakeholders to ensure resource capacity and strategic alignment to meet channel needs Support effective distribution execution by providing the right tools/processes and building the right knowledge Serve as SME for operational processes and best practices serving the needs of Key Markets partners Act as the business owner for bringing new opportunities to market Articulate channel needs and influence support across organizational initiatives to ensure channel needs are met for new capabilities and solutions Partner with client management to expand upon solutions leveraged in market to drive employer and member engagement in benefits Facilitate the need for expanded technical and integration capabilities Engage on high profile partner initiatives as needed You Have: Minimum of 8 years in distribution facing operations roles for a multi-faceted corporation (insurance industry preferred). Deep expertise in specialty and alternative distribution models and associated operational needs. Proven success in designing and implementing innovative strategies to enhance the customer experience in a digital consumer-centric ecosystem. A strong process and system orientation and an ability to identify impacts of change while optimizing business value. Strong general management mindset and experience with broad functional strategy development and execution. Commercial insurance, financial services and/or management consulting experience preferred. Strong background in business case development and execution. High energy with strong executive presence and public speaking skills including presentation to C-Suite, as well as field stakeholders. Relentless focus on innovative strategic thought leadership and a track record of success in affecting change, having delivered quantifiable impact on company revenue. Compelling presentation skills e.g. comfortable speaking at large group conferences and webinars. Location, Work Arrangement, and Travel: Preferred locations for this position include New York, NY; Holmdel, NJ; Boston, MA; and Bethlehem, PA. The work arrangement will be hybrid (three days per week in a local Guardian Office; two days working from home). Approximately 10-15% travel associated with this position. Salary Range: $118,980.00 - $195,465.00 The salary range reflected above is a good faith estimate of base pay for the primary location of the position. The salary for this position ultimately will be determined based on the education, experience, knowledge, and abilities of the successful candidate. In addition to salary, this role may also be eligible for annual, sales, or other incentive compensation. Our Promise At Guardian, you’ll have the support and flexibility to achieve your professional and personal goals.  Through skill-building, leadership development and philanthropic opportunities, we provide opportunities to build communities and grow your career, surrounded by diverse colleagues with high ethical standards. Inspire Well-Being As part of Guardian’s Purpose – to inspire well-being – we are committed to offering contemporary, supportive, flexible, and inclusive benefits and resources to our colleagues. Explore our company benefits at www.guardianlife.com/careers/corporate/benefits . Benefits apply to full-time eligible employees. Interns are not eligible for most Company benefits. Equal Employment Opportunity Guardian is an equal opportunity employer. All qualified applicants will be considered for employment without regard to age, race, color, creed, religion, sex, affectional or sexual orientation, national origin, ancestry, marital status, disability, military or veteran status, or any other classification protected by applicable law. Accommodations Guardian is committed to providing access, equal opportunity and reasonable accommodation for individuals with disabilities in employment, its services, programs, and activities. Guardian also provides reasonable accommodations to qualified job applicants (and employees) to accommodate the individual's known limitations related to pregnancy, childbirth, or related medical conditions, unless doing so would create an undue hardship. If reasonable accommodation is needed to participate in the job application or interview process, to perform essential job functions, and/or to receive other benefits and privileges of employment, please contact MyHR@glic.com. Please note: this resource is for accommodation requests only. For all other inquires related to your application and careers at Guardian, refer to the Guardian Careers site. Visa Sponsorship Guardian is not currently or in the foreseeable future sponsoring employment visas.  In order to be a successful applicant. you must be legally authorized to work in the United States, without the need for employer sponsorship. Current Guardian Colleagues: Please apply through the internal Jobs Hub in Workday.</t>
         </is>
       </c>
       <c r="D28" s="3" t="inlineStr">
         <is>
-          <t>Atlanta - Regional Office</t>
-        </is>
-      </c>
-      <c r="E28" s="3" t="inlineStr"/>
+          <t>New York</t>
+        </is>
+      </c>
+      <c r="E28" s="3" t="inlineStr">
+        <is>
+          <t>Bethlehem, Boston, Holmdel</t>
+        </is>
+      </c>
       <c r="F28" s="3" t="inlineStr">
         <is>
           <t>2026-02-12</t>
@@ -1694,17 +1698,17 @@
       </c>
       <c r="G28" s="3" t="inlineStr">
         <is>
-          <t>R000108402</t>
+          <t>R000108155</t>
         </is>
       </c>
       <c r="H28" s="3" t="inlineStr">
         <is>
-          <t>Fully Remote</t>
+          <t>Hybrid - In office 3 days per week</t>
         </is>
       </c>
       <c r="I28" s="3" t="inlineStr">
         <is>
-          <t>https://guardianlife.wd5.myworkdayjobs.com/Guardian-Life-Careers/job/Atlanta---Regional-Office/Associate-Sales-Representative--Group-Benefits_R000108402</t>
+          <t>https://guardianlife.wd5.myworkdayjobs.com/Guardian-Life-Careers/job/New-York/Key-Markets-Strategy---Operations-Lead--Group-Benefits_R000108155</t>
         </is>
       </c>
     </row>
@@ -1716,28 +1720,28 @@
       </c>
       <c r="B29" s="4" t="inlineStr">
         <is>
-          <t>Client Manager, Group Benefits - Premier Accounts</t>
+          <t>Associate Sales Representative, Group Benefits</t>
         </is>
       </c>
       <c r="C29" s="4" t="inlineStr">
         <is>
-          <t>As the Client Manager, Group Benefits - Premier Accounts, you will be the main contact for our Premier Account client relationships. This role is directly accountable for client retention, satisfaction, and enhancing the client experience. You will be responsible for persistence, growth, and profitability of your book of business through relationship development with clients, brokers, and key internal stakeholders. Client management and negotiation skills are essential for this role.   Do you have a passion for doing the right thing for customers and making their experience the best they could possibly imagine?  Are you a team player who is adept at collaborating across internal teams?  Is a culture where “People Count,” “We Do the Right Thing,” and “We Hold Ourselves to Very High Standards” important to you? You are Well versed on consultative selling skills, negotiation skills, and the ability to influence and persuade. Comfortable with virtual communication, presentation, consultative selling, and relationship building A team player with ability to build relationships and effectively interact both internally and externally with individuals at all levels of the organization and customer orientation. Able to collaborate across internal teams including collaborative selling. Strategic and critical thinking and basic math skills Open to change and new ways of working,  specifically including the ability to execute new strategies/tactics to drive results Able to exercise sound judgment and manage conflict. Able to exude confidence and demonstrate optimism and positive attitude. Advanced in organizational and time management skills. You will Assume overall responsibility for management of clients (100-1999 lives) with the objective of ensuring that client satisfaction, persistency, growth, and profitability goals are achieved. Oversight of the account, building strong relationships with clients and brokers/consultants. Work closely with internal partners to gain  buy-in for the account management strategy and position. Strategically manage the lifecycle of a client to drive the right solutions to their benefit needs Balance the needs of the client with those of the business. Achieve yearly financial growth goals You have BA or BS degree preferred or equivalent work experience. Minimum of 3 years experience in account management, sales. Group insurance experience preferred. Demonstrated success in dealing with brokers/consultants as well as sophisticated clients. Ability to analyze data to influence and execute on renewal decisions along with deploying the right solutions for the client. Ability to leverage all sales enablement technology, training, and tools with proficiency in key technology platforms:  Microsoft Office suite: PowerPoint, Word, Outlook, Teams; Tableau, Salesforce. Ability to flex environments, operating &amp; building rapport effectively both in virtual and live environments Ability to adapt to changes in a fast paced and dynamic environment. Depth of experience and knowledge of relevant industry products and processes including, but not limited to Worksite, LTD, Dental products and absence management, online enrollment, experience rating, dental network analysis processes. Must achieve required industry licensing within 90 days of date of hire and maintain license through completing Continuing Education requirements. Location Must reside in the Dallas/Fort Worth, TX area as you will be in office 1 day a week. Up to 25% travel within U.S Salary Range: $53,490.00 - $87,870.00 The salary range reflected above is a good faith estimate of base pay for the primary location of the position. The salary for this position ultimately will be determined based on the education, experience, knowledge, and abilities of the successful candidate. In addition to salary, this role may also be eligible for annual, sales, or other incentive compensation. Our Promise At Guardian, you’ll have the support and flexibility to achieve your professional and personal goals.  Through skill-building, leadership development and philanthropic opportunities, we provide opportunities to build communities and grow your career, surrounded by diverse colleagues with high ethical standards. Inspire Well-Being As part of Guardian’s Purpose – to inspire well-being – we are committed to offering contemporary, supportive, flexible, and inclusive benefits and resources to our colleagues. Explore our company benefits at www.guardianlife.com/careers/corporate/benefits . Benefits apply to full-time eligible employees. Interns are not eligible for most Company benefits. Equal Employment Opportunity Guardian is an equal opportunity employer. All qualified applicants will be considered for employment without regard to age, race, color, creed, religion, sex, affectional or sexual orientation, national origin, ancestry, marital status, disability, military or veteran status, or any other classification protected by applicable law. Accommodations Guardian is committed to providing access, equal opportunity and reasonable accommodation for individuals with disabilities in employment, its services, programs, and activities. Guardian also provides reasonable accommodations to qualified job applicants (and employees) to accommodate the individual's known limitations related to pregnancy, childbirth, or related medical conditions, unless doing so would create an undue hardship. If reasonable accommodation is needed to participate in the job application or interview process, to perform essential job functions, and/or to receive other benefits and privileges of employment, please contact MyHR@glic.com. Please note: this resource is for accommodation requests only. For all other inquires related to your application and careers at Guardian, refer to the Guardian Careers site. Visa Sponsorship Guardian is not currently or in the foreseeable future sponsoring employment visas.  In order to be a successful applicant. you must be legally authorized to work in the United States, without the need for employer sponsorship. Current Guardian Colleagues: Please apply through the internal Jobs Hub in Workday.</t>
+          <t>Guardian's Group Benefits team is seeking Associate Sales Representative who will be responsible for building and maintaining brokers and plan holder relationships to drive ongoing sales and retention of groups of 2-2,000 lives with a primary focus on the under 100 lives market. Success will be determined based on the ability to attain high levels of production through broker development and internal relationships. This role will report to the Market Leader within the assigned territory. You Will: Market, position, and sell Guardian’s entire Group Benefits portfolio products and technology solutions to your designated brokers. This includes Dental, Vision, Life, Disability, Absence, and Supplemental Health products. Support the general wellbeing of the broker and client relationship for the development and growth of Guardian sales and client retention. Understand territory dynamics to build, develop and maintain broker relationships to grow the book of business while representing Guardian’s vision to inspire well-being. Be accountable for consistently achieving or exceeding personal sales production expectations by having a clear understanding of products. Identify, recommend and champion process improvements and organizational initiatives to increase sales of product offerings. Achieve required industry licensing within 90 days of date of hire and maintain license through completing Continuing Education requirements. You Have: A BA/BS degree or equivalent work experience Ability to consistently achieve or exceed personal sales production expectations established by management, as stated in the Market business plan that is consistent with Group Profit Center objectives. Soft Skills: Collaborative team player with the ability to effectively build rapport in person and virtually. Exercise sound judgement and integrity in a changing, matrixed, and fast past environment. Exude confidence, positivity, and proactivity. Act with accountability to deliver on commitments with speed and quality. Location and Travel Requirements: Successful hire must be based in the Atlanta, GA area Up to 20% travel within the U.S. Salary: $35,000 ​ The salary reflected above is a good faith estimate of base pay for the primary location of the position. The salary for this position ultimately will be determined based on the education, experience, knowledge, and abilities of the successful candidate. In addition to salary, this role may also be eligible for annual, sales, or other incentive compensation. Our Promise At Guardian, you’ll have the support and flexibility to achieve your professional and personal goals.  Through skill-building, leadership development and philanthropic opportunities, we provide opportunities to build communities and grow your career, surrounded by diverse colleagues with high ethical standards. Inspire Well-Being As part of Guardian’s Purpose – to inspire well-being – we are committed to offering contemporary, supportive, flexible, and inclusive benefits and resources to our colleagues. Explore our company benefits at www.guardianlife.com/careers/corporate/benefits . Benefits apply to full-time eligible employees. Interns are not eligible for most Company benefits. Equal Employment Opportunity Guardian is an equal opportunity employer. All qualified applicants will be considered for employment without regard to age, race, color, creed, religion, sex, affectional or sexual orientation, national origin, ancestry, marital status, disability, military or veteran status, or any other classification protected by applicable law. Accommodations Guardian is committed to providing access, equal opportunity and reasonable accommodation for individuals with disabilities in employment, its services, programs, and activities. Guardian also provides reasonable accommodations to qualified job applicants (and employees) to accommodate the individual's known limitations related to pregnancy, childbirth, or related medical conditions, unless doing so would create an undue hardship. If reasonable accommodation is needed to participate in the job application or interview process, to perform essential job functions, and/or to receive other benefits and privileges of employment, please contact MyHR@glic.com. Please note: this resource is for accommodation requests only. For all other inquires related to your application and careers at Guardian, refer to the Guardian Careers site. Visa Sponsorship Guardian is not currently or in the foreseeable future sponsoring employment visas.  In order to be a successful applicant. you must be legally authorized to work in the United States, without the need for employer sponsorship. Current Guardian Colleagues: Please apply through the internal Jobs Hub in Workday</t>
         </is>
       </c>
       <c r="D29" s="4" t="inlineStr">
         <is>
-          <t>Work From Home - TX</t>
+          <t>Atlanta - Regional Office</t>
         </is>
       </c>
       <c r="E29" s="4" t="inlineStr"/>
       <c r="F29" s="4" t="inlineStr">
         <is>
-          <t>2026-02-11</t>
+          <t>2026-02-12</t>
         </is>
       </c>
       <c r="G29" s="4" t="inlineStr">
         <is>
-          <t>R000108604</t>
+          <t>R000108402</t>
         </is>
       </c>
       <c r="H29" s="4" t="inlineStr">
@@ -1747,7 +1751,7 @@
       </c>
       <c r="I29" s="4" t="inlineStr">
         <is>
-          <t>https://guardianlife.wd5.myworkdayjobs.com/Guardian-Life-Careers/job/Work-From-Home---TX/Client-Manager--Group-Benefits---Premier-Accounts_R000108604</t>
+          <t>https://guardianlife.wd5.myworkdayjobs.com/Guardian-Life-Careers/job/Atlanta---Regional-Office/Associate-Sales-Representative--Group-Benefits_R000108402</t>
         </is>
       </c>
     </row>
@@ -1759,24 +1763,20 @@
       </c>
       <c r="B30" s="3" t="inlineStr">
         <is>
-          <t>Life Claims Specialist, FPRS (Financial Protection and Retirement Solutions)</t>
+          <t>Client Manager, Group Benefits - Premier Accounts</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr">
         <is>
-          <t>As the Life Claims Specialist, FPRS (Financial Protection and Retirement Solutions), you will play a key role in delivering meaningful experiences that support growth—both for your career and for our team’s collective future. At Guardian, we live our Purpose every day. As champions of wellbeing for ourselves, our communities, and our consumers, we work together to turn what’s possible into reality. We believe in your aspirations for purpose, leadership, and achievement in both your professional and personal life, and this role provides the opportunity to bring those aspirations to life. We will help build the core competencies you will need to be a successful Life Claims Specialist. In your first year, we will provide extensive training in a highly supportive environment. If you have an internal drive to investigate using your critical thinking skills, assessing policy matters, and can manage competing priorities while meeting deadlines, this is your opportunity to make a difference, grow your career, and be a part of moving the organization into the future. You will Be responsible for timely and accurate adjudication of FPRS (Financial Protection and Retirement Solutions) life claims. Work within a team providing strong customer service making timely, but thoughtful decisions to achieve a claim determination. Review policy language and other claim documentation Work within a team-driven and customer-focused environment Maintain composure and direction in high pressure situations. Develop and enhance your communication skills to meet the customer’s needs, while demonstrating empathy, flexibility, responsiveness, and an action-oriented approach Develop critical thinking to issue spot and identify resources needed to assist in making claim determinations. You have A college or university degree or the equivalent work experience that provides knowledge and exposure to claims, service or other principles and concepts. At least two years of claim related work experience (Individual Life Claims preferred) Experience and an interest in providing quality customer service both written and telephonic. Strong analytical skills, with attention to detail Strong written and verbal communication skills Demonstrated experience prioritizing competing priorities with deadlines. Working knowledge of Microsoft Office products, including Word, Excel, and Outlook Location /Travel This is a hybrid role. If you are within close proximity to one of our Guardian hubs—Bethlehem, PA; Pittsfield, MA; New York City; or Boston, MA—we prefer that you work in the office three days per week , with Bethlehem or Pittsfield strongly preferred . Salary Range: $50,260.00 - $75,385.00 The salary range reflected above is a good faith estimate of base pay for the primary location of the position. The salary for this position ultimately will be determined based on the education, experience, knowledge, and abilities of the successful candidate. In addition to salary, this role may also be eligible for annual, sales, or other incentive compensation. Our Promise At Guardian, you’ll have the support and flexibility to achieve your professional and personal goals.  Through skill-building, leadership development and philanthropic opportunities, we provide opportunities to build communities and grow your career, surrounded by diverse colleagues with high ethical standards. Inspire Well-Being As part of Guardian’s Purpose – to inspire well-being – we are committed to offering contemporary, supportive, flexible, and inclusive benefits and resources to our colleagues. Explore our company benefits at www.guardianlife.com/careers/corporate/benefits . Benefits apply to full-time eligible employees. Interns are not eligible for most Company benefits. Equal Employment Opportunity Guardian is an equal opportunity employer. All qualified applicants will be considered for employment without regard to age, race, color, creed, religion, sex, affectional or sexual orientation, national origin, ancestry, marital status, disability, military or veteran status, or any other classification protected by applicable law. Accommodations Guardian is committed to providing access, equal opportunity and reasonable accommodation for individuals with disabilities in employment, its services, programs, and activities. Guardian also provides reasonable accommodations to qualified job applicants (and employees) to accommodate the individual's known limitations related to pregnancy, childbirth, or related medical conditions, unless doing so would create an undue hardship. If reasonable accommodation is needed to participate in the job application or interview process, to perform essential job functions, and/or to receive other benefits and privileges of employment, please contact MyHR@glic.com. Please note: this resource is for accommodation requests only. For all other inquires related to your application and careers at Guardian, refer to the Guardian Careers site. Visa Sponsorship Guardian is not currently or in the foreseeable future sponsoring employment visas.  In order to be a successful applicant. you must be legally authorized to work in the United States, without the need for employer sponsorship. Current Guardian Colleagues: Please apply through the internal Jobs Hub in Workday.</t>
+          <t>As the Client Manager, Group Benefits - Premier Accounts, you will be the main contact for our Premier Account client relationships. This role is directly accountable for client retention, satisfaction, and enhancing the client experience. You will be responsible for persistence, growth, and profitability of your book of business through relationship development with clients, brokers, and key internal stakeholders. Client management and negotiation skills are essential for this role.   Do you have a passion for doing the right thing for customers and making their experience the best they could possibly imagine?  Are you a team player who is adept at collaborating across internal teams?  Is a culture where “People Count,” “We Do the Right Thing,” and “We Hold Ourselves to Very High Standards” important to you? You are Well versed on consultative selling skills, negotiation skills, and the ability to influence and persuade. Comfortable with virtual communication, presentation, consultative selling, and relationship building A team player with ability to build relationships and effectively interact both internally and externally with individuals at all levels of the organization and customer orientation. Able to collaborate across internal teams including collaborative selling. Strategic and critical thinking and basic math skills Open to change and new ways of working,  specifically including the ability to execute new strategies/tactics to drive results Able to exercise sound judgment and manage conflict. Able to exude confidence and demonstrate optimism and positive attitude. Advanced in organizational and time management skills. You will Assume overall responsibility for management of clients (100-1999 lives) with the objective of ensuring that client satisfaction, persistency, growth, and profitability goals are achieved. Oversight of the account, building strong relationships with clients and brokers/consultants. Work closely with internal partners to gain  buy-in for the account management strategy and position. Strategically manage the lifecycle of a client to drive the right solutions to their benefit needs Balance the needs of the client with those of the business. Achieve yearly financial growth goals You have BA or BS degree preferred or equivalent work experience. Minimum of 3 years experience in account management, sales. Group insurance experience preferred. Demonstrated success in dealing with brokers/consultants as well as sophisticated clients. Ability to analyze data to influence and execute on renewal decisions along with deploying the right solutions for the client. Ability to leverage all sales enablement technology, training, and tools with proficiency in key technology platforms:  Microsoft Office suite: PowerPoint, Word, Outlook, Teams; Tableau, Salesforce. Ability to flex environments, operating &amp; building rapport effectively both in virtual and live environments Ability to adapt to changes in a fast paced and dynamic environment. Depth of experience and knowledge of relevant industry products and processes including, but not limited to Worksite, LTD, Dental products and absence management, online enrollment, experience rating, dental network analysis processes. Must achieve required industry licensing within 90 days of date of hire and maintain license through completing Continuing Education requirements. Location Must reside in the Dallas/Fort Worth, TX area as you will be in office 1 day a week. Up to 25% travel within U.S Salary Range: $53,490.00 - $87,870.00 The salary range reflected above is a good faith estimate of base pay for the primary location of the position. The salary for this position ultimately will be determined based on the education, experience, knowledge, and abilities of the successful candidate. In addition to salary, this role may also be eligible for annual, sales, or other incentive compensation. Our Promise At Guardian, you’ll have the support and flexibility to achieve your professional and personal goals.  Through skill-building, leadership development and philanthropic opportunities, we provide opportunities to build communities and grow your career, surrounded by diverse colleagues with high ethical standards. Inspire Well-Being As part of Guardian’s Purpose – to inspire well-being – we are committed to offering contemporary, supportive, flexible, and inclusive benefits and resources to our colleagues. Explore our company benefits at www.guardianlife.com/careers/corporate/benefits . Benefits apply to full-time eligible employees. Interns are not eligible for most Company benefits. Equal Employment Opportunity Guardian is an equal opportunity employer. All qualified applicants will be considered for employment without regard to age, race, color, creed, religion, sex, affectional or sexual orientation, national origin, ancestry, marital status, disability, military or veteran status, or any other classification protected by applicable law. Accommodations Guardian is committed to providing access, equal opportunity and reasonable accommodation for individuals with disabilities in employment, its services, programs, and activities. Guardian also provides reasonable accommodations to qualified job applicants (and employees) to accommodate the individual's known limitations related to pregnancy, childbirth, or related medical conditions, unless doing so would create an undue hardship. If reasonable accommodation is needed to participate in the job application or interview process, to perform essential job functions, and/or to receive other benefits and privileges of employment, please contact MyHR@glic.com. Please note: this resource is for accommodation requests only. For all other inquires related to your application and careers at Guardian, refer to the Guardian Careers site. Visa Sponsorship Guardian is not currently or in the foreseeable future sponsoring employment visas.  In order to be a successful applicant. you must be legally authorized to work in the United States, without the need for employer sponsorship. Current Guardian Colleagues: Please apply through the internal Jobs Hub in Workday.</t>
         </is>
       </c>
       <c r="D30" s="3" t="inlineStr">
         <is>
-          <t>Bethlehem</t>
-        </is>
-      </c>
-      <c r="E30" s="3" t="inlineStr">
-        <is>
-          <t>New York, Boston, Pittsfield, Holmdel</t>
-        </is>
-      </c>
+          <t>Work From Home - TX</t>
+        </is>
+      </c>
+      <c r="E30" s="3" t="inlineStr"/>
       <c r="F30" s="3" t="inlineStr">
         <is>
           <t>2026-02-11</t>
@@ -1784,17 +1784,17 @@
       </c>
       <c r="G30" s="3" t="inlineStr">
         <is>
-          <t>R000108590</t>
+          <t>R000108604</t>
         </is>
       </c>
       <c r="H30" s="3" t="inlineStr">
         <is>
-          <t>Hybrid - In office 3 days per week</t>
+          <t>Fully Remote</t>
         </is>
       </c>
       <c r="I30" s="3" t="inlineStr">
         <is>
-          <t>https://guardianlife.wd5.myworkdayjobs.com/Guardian-Life-Careers/job/Bethlehem/FPRS--financial-protection-and-retirement-services----Life-Claims-Specialist_R000108590-1</t>
+          <t>https://guardianlife.wd5.myworkdayjobs.com/Guardian-Life-Careers/job/Work-From-Home---TX/Client-Manager--Group-Benefits---Premier-Accounts_R000108604</t>
         </is>
       </c>
     </row>
@@ -1806,12 +1806,12 @@
       </c>
       <c r="B31" s="4" t="inlineStr">
         <is>
-          <t>Annuity Operations Care Specialist</t>
+          <t>Life Claims Specialist, FPRS (Financial Protection and Retirement Solutions)</t>
         </is>
       </c>
       <c r="C31" s="4" t="inlineStr">
         <is>
-          <t>Guardian’s Annuity In-Force Operations CARE team is seeking a highly motivated individual who is pursuing an opportunity to develop and grow their experience as an Annuity Operations Specialist . We are looking for an avid learner who possesses strong analytical and communication skills to support our annuity growth. This role is responsible for delivering accurate, timely, and compliant processing to support end-to-end in-force annuity transactions. As well as providing a high-touch service experience to our customers. As an Operations Specialist, you are empowered to take full ownership of each request from intake through resolution. You ensure stakeholders are informed at every stage, resolve complex issues independently, and escalate when appropriate to meet service and regulatory expectations. This role embraces the CARE mindset — Communicate, Advocate, Respond, and Empower — demonstrating authentic care for contract holders, field partners, and internal teams while driving operational excellence. You are Motivated to positively impact customer and partner experiences through accurate in-force transaction processing Action-oriented with the ability to assess priorities and manage competing deadlines Detail-oriented and procedure-driven with a strong commitment to quality and compliance Comfortable communicating complex information clearly via email and phone Accountable for outcomes and follow-through Willing to challenge existing processes and contribute ideas for improvement A collaborative team member open to feedback Flexible to contribute overtime equitably when needed You will Process and prioritize a wide range of in-force annuity transactions Provide high-level service to contract holders and internal partners Own complex or escalated in-force cases from intake to resolution Perform root-cause analysis on issues and recommend improvements Meet or exceed quality, accuracy, and timeliness metrics Partner with Product, Compliance, Finance, Treasury, and Contact Center teams Develop subject-matter expertise in annuity products, systems, and procedures Participate in cross-functional projects and initiatives You have College degree preferred or equivalent industry experience 2+ years of insurance, annuity, or retirement operations experience Working knowledge of annuity products preferred Strong organizational skills and attention to detail Ability to exercise discretion and independent judgment Proficiency in Microsoft Outlook, Word, and Excel preferred A positive, service-oriented mindset and commitment to continuous learning LOCATION This is a hybrid role, requiring three days per week onsite in either Bethlehem, PA or Pittsfield, MA office. Team members must be able to come to campus as needed. Onsite requirements are subject to change based on business needs. TRAVEL No travel is required for this position. Salary Range: $42,830.00 - $64,250.00 The salary range reflected above is a good faith estimate of base pay for the primary location of the position. The salary for this position ultimately will be determined based on the education, experience, knowledge, and abilities of the successful candidate. In addition to salary, this role may also be eligible for annual, sales, or other incentive compensation. Our Promise At Guardian, you’ll have the support and flexibility to achieve your professional and personal goals.  Through skill-building, leadership development and philanthropic opportunities, we provide opportunities to build communities and grow your career, surrounded by diverse colleagues with high ethical standards. Inspire Well-Being As part of Guardian’s Purpose – to inspire well-being – we are committed to offering contemporary, supportive, flexible, and inclusive benefits and resources to our colleagues. Explore our company benefits at www.guardianlife.com/careers/corporate/benefits . Benefits apply to full-time eligible employees. Interns are not eligible for most Company benefits. Equal Employment Opportunity Guardian is an equal opportunity employer. All qualified applicants will be considered for employment without regard to age, race, color, creed, religion, sex, affectional or sexual orientation, national origin, ancestry, marital status, disability, military or veteran status, or any other classification protected by applicable law. Accommodations Guardian is committed to providing access, equal opportunity and reasonable accommodation for individuals with disabilities in employment, its services, programs, and activities. Guardian also provides reasonable accommodations to qualified job applicants (and employees) to accommodate the individual's known limitations related to pregnancy, childbirth, or related medical conditions, unless doing so would create an undue hardship. If reasonable accommodation is needed to participate in the job application or interview process, to perform essential job functions, and/or to receive other benefits and privileges of employment, please contact MyHR@glic.com. Please note: this resource is for accommodation requests only. For all other inquires related to your application and careers at Guardian, refer to the Guardian Careers site. Visa Sponsorship Guardian is not currently or in the foreseeable future sponsoring employment visas.  In order to be a successful applicant. you must be legally authorized to work in the United States, without the need for employer sponsorship. Current Guardian Colleagues: Please apply through the internal Jobs Hub in Workday.</t>
+          <t>As the Life Claims Specialist, FPRS (Financial Protection and Retirement Solutions), you will play a key role in delivering meaningful experiences that support growth—both for your career and for our team’s collective future. At Guardian, we live our Purpose every day. As champions of wellbeing for ourselves, our communities, and our consumers, we work together to turn what’s possible into reality. We believe in your aspirations for purpose, leadership, and achievement in both your professional and personal life, and this role provides the opportunity to bring those aspirations to life. We will help build the core competencies you will need to be a successful Life Claims Specialist. In your first year, we will provide extensive training in a highly supportive environment. If you have an internal drive to investigate using your critical thinking skills, assessing policy matters, and can manage competing priorities while meeting deadlines, this is your opportunity to make a difference, grow your career, and be a part of moving the organization into the future. You will Be responsible for timely and accurate adjudication of FPRS (Financial Protection and Retirement Solutions) life claims. Work within a team providing strong customer service making timely, but thoughtful decisions to achieve a claim determination. Review policy language and other claim documentation Work within a team-driven and customer-focused environment Maintain composure and direction in high pressure situations. Develop and enhance your communication skills to meet the customer’s needs, while demonstrating empathy, flexibility, responsiveness, and an action-oriented approach Develop critical thinking to issue spot and identify resources needed to assist in making claim determinations. You have A college or university degree or the equivalent work experience that provides knowledge and exposure to claims, service or other principles and concepts. At least two years of claim related work experience (Individual Life Claims preferred) Experience and an interest in providing quality customer service both written and telephonic. Strong analytical skills, with attention to detail Strong written and verbal communication skills Demonstrated experience prioritizing competing priorities with deadlines. Working knowledge of Microsoft Office products, including Word, Excel, and Outlook Location /Travel This is a hybrid role. If you are within close proximity to one of our Guardian hubs—Bethlehem, PA; Pittsfield, MA; New York City; or Boston, MA—we prefer that you work in the office three days per week , with Bethlehem or Pittsfield strongly preferred . Salary Range: $50,260.00 - $75,385.00 The salary range reflected above is a good faith estimate of base pay for the primary location of the position. The salary for this position ultimately will be determined based on the education, experience, knowledge, and abilities of the successful candidate. In addition to salary, this role may also be eligible for annual, sales, or other incentive compensation. Our Promise At Guardian, you’ll have the support and flexibility to achieve your professional and personal goals.  Through skill-building, leadership development and philanthropic opportunities, we provide opportunities to build communities and grow your career, surrounded by diverse colleagues with high ethical standards. Inspire Well-Being As part of Guardian’s Purpose – to inspire well-being – we are committed to offering contemporary, supportive, flexible, and inclusive benefits and resources to our colleagues. Explore our company benefits at www.guardianlife.com/careers/corporate/benefits . Benefits apply to full-time eligible employees. Interns are not eligible for most Company benefits. Equal Employment Opportunity Guardian is an equal opportunity employer. All qualified applicants will be considered for employment without regard to age, race, color, creed, religion, sex, affectional or sexual orientation, national origin, ancestry, marital status, disability, military or veteran status, or any other classification protected by applicable law. Accommodations Guardian is committed to providing access, equal opportunity and reasonable accommodation for individuals with disabilities in employment, its services, programs, and activities. Guardian also provides reasonable accommodations to qualified job applicants (and employees) to accommodate the individual's known limitations related to pregnancy, childbirth, or related medical conditions, unless doing so would create an undue hardship. If reasonable accommodation is needed to participate in the job application or interview process, to perform essential job functions, and/or to receive other benefits and privileges of employment, please contact MyHR@glic.com. Please note: this resource is for accommodation requests only. For all other inquires related to your application and careers at Guardian, refer to the Guardian Careers site. Visa Sponsorship Guardian is not currently or in the foreseeable future sponsoring employment visas.  In order to be a successful applicant. you must be legally authorized to work in the United States, without the need for employer sponsorship. Current Guardian Colleagues: Please apply through the internal Jobs Hub in Workday.</t>
         </is>
       </c>
       <c r="D31" s="4" t="inlineStr">
@@ -1821,17 +1821,17 @@
       </c>
       <c r="E31" s="4" t="inlineStr">
         <is>
-          <t>Pittsfield</t>
+          <t>New York, Boston, Pittsfield, Holmdel</t>
         </is>
       </c>
       <c r="F31" s="4" t="inlineStr">
         <is>
-          <t>2026-02-10</t>
+          <t>2026-02-11</t>
         </is>
       </c>
       <c r="G31" s="4" t="inlineStr">
         <is>
-          <t>R000108593</t>
+          <t>R000108590</t>
         </is>
       </c>
       <c r="H31" s="4" t="inlineStr">
@@ -1841,7 +1841,7 @@
       </c>
       <c r="I31" s="4" t="inlineStr">
         <is>
-          <t>https://guardianlife.wd5.myworkdayjobs.com/Guardian-Life-Careers/job/Bethlehem/Annuity-Operations-Care-Specialist_R000108593</t>
+          <t>https://guardianlife.wd5.myworkdayjobs.com/Guardian-Life-Careers/job/Bethlehem/FPRS--financial-protection-and-retirement-services----Life-Claims-Specialist_R000108590-1</t>
         </is>
       </c>
     </row>
@@ -1853,12 +1853,12 @@
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>Lead, Payroll Specialist</t>
+          <t>Annuity Operations Care Specialist</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr">
         <is>
-          <t>Is the opportunity to join a culture where “We Do the Right Thing,” and “We Courageously Shape Our Future Together” important to you? If so, Guardian is seeking a talented and motivated individual to join our team as a Lead, Payroll Specialist. This role will ensure that all payroll administration and accounting processes are regularly evaluated to be as streamlined and efficient as possible. It will be vital to ensure accuracy and timeliness response to ensure an ideal colleague experience across Guardian businesses. You will: Administer payroll for multiple schedules, ensuring timely and accurate compensation for all employees. Maintain payroll controls and procedures to support accuracy and safeguard sensitive information. Assist with wage garnishment vendor management, including processing orders and communicating with vendors. Streamline payroll processes to improve efficiency and reduce errors. Prepare third-party payment requests related to payroll deductions and statutory obligations. Collaborate with related departments to resolve payroll issues and support organizational goals. Serve as a Tier 3 payroll authority by addressing complex payroll questions and escalations. Support accounting functions through accurate payroll reporting and reconciliation. Crosstrain payroll staff to ensure team coverage and continuity of operations. You have: Strong proficiency with Workday Payroll module (required). Knowledge of Workday HCM a plus. Minimum of 4 years of demonstrated experience in payroll functions. Ability to function as a working (hands-on) payroll lead processing payroll, as well as cover for team members in back-up role for vacation and/or high-volume work efforts. Strong focus on customer service, working as a supportive escalation expert to the HR Shared Services Center and a valued partner to other COEs and HR Business Partners as required. Ability to manage sensitive information, working with internal partners to accomplish objectives without compromising a high threshold for discretion and confidentiality. Highly autonomous and self-motivated, demonstrating sound judgment and initiative while keeping others informed as appropriate. Time management skills to successfully prioritize multiple projects at a given time. Strong skills in Microsoft Office applications, especially MS Word and MS Excel. Knowledge of payroll administration, controls, governance, and accounting best practices with established network for keeping current including but not limited to multi-state payroll practices, requirements, and financial/tax implications. Understanding of current federal, state, and local regulatory and compliance obligations related to payroll and how to fulfil them in a timely and accurate manner. Reporting Relationship This position reports to the Head of Payroll who then reports to the Head of HR Service Delivery. Location: Hybrid role: 3 days in Bethlehem, PA office. 2 days WFH. Salary Range: $68,970.00 - $113,310.00 The salary range reflected above is a good faith estimate of base pay for the primary location of the position. The salary for this position ultimately will be determined based on the education, experience, knowledge, and abilities of the successful candidate. In addition to salary, this role may also be eligible for annual, sales, or other incentive compensation. Our Promise At Guardian, you’ll have the support and flexibility to achieve your professional and personal goals.  Through skill-building, leadership development and philanthropic opportunities, we provide opportunities to build communities and grow your career, surrounded by diverse colleagues with high ethical standards. Inspire Well-Being As part of Guardian’s Purpose – to inspire well-being – we are committed to offering contemporary, supportive, flexible, and inclusive benefits and resources to our colleagues. Explore our company benefits at www.guardianlife.com/careers/corporate/benefits . Benefits apply to full-time eligible employees. Interns are not eligible for most Company benefits. Equal Employment Opportunity Guardian is an equal opportunity employer. All qualified applicants will be considered for employment without regard to age, race, color, creed, religion, sex, affectional or sexual orientation, national origin, ancestry, marital status, disability, military or veteran status, or any other classification protected by applicable law. Accommodations Guardian is committed to providing access, equal opportunity and reasonable accommodation for individuals with disabilities in employment, its services, programs, and activities. Guardian also provides reasonable accommodations to qualified job applicants (and employees) to accommodate the individual's known limitations related to pregnancy, childbirth, or related medical conditions, unless doing so would create an undue hardship. If reasonable accommodation is needed to participate in the job application or interview process, to perform essential job functions, and/or to receive other benefits and privileges of employment, please contact MyHR@glic.com. Please note: this resource is for accommodation requests only. For all other inquires related to your application and careers at Guardian, refer to the Guardian Careers site. Visa Sponsorship Guardian is not currently or in the foreseeable future sponsoring employment visas.  In order to be a successful applicant. you must be legally authorized to work in the United States, without the need for employer sponsorship. Current Guardian Colleagues: Please apply through the internal Jobs Hub in Workday.</t>
+          <t>Guardian’s Annuity In-Force Operations CARE team is seeking a highly motivated individual who is pursuing an opportunity to develop and grow their experience as an Annuity Operations Specialist . We are looking for an avid learner who possesses strong analytical and communication skills to support our annuity growth. This role is responsible for delivering accurate, timely, and compliant processing to support end-to-end in-force annuity transactions. As well as providing a high-touch service experience to our customers. As an Operations Specialist, you are empowered to take full ownership of each request from intake through resolution. You ensure stakeholders are informed at every stage, resolve complex issues independently, and escalate when appropriate to meet service and regulatory expectations. This role embraces the CARE mindset — Communicate, Advocate, Respond, and Empower — demonstrating authentic care for contract holders, field partners, and internal teams while driving operational excellence. You are Motivated to positively impact customer and partner experiences through accurate in-force transaction processing Action-oriented with the ability to assess priorities and manage competing deadlines Detail-oriented and procedure-driven with a strong commitment to quality and compliance Comfortable communicating complex information clearly via email and phone Accountable for outcomes and follow-through Willing to challenge existing processes and contribute ideas for improvement A collaborative team member open to feedback Flexible to contribute overtime equitably when needed You will Process and prioritize a wide range of in-force annuity transactions Provide high-level service to contract holders and internal partners Own complex or escalated in-force cases from intake to resolution Perform root-cause analysis on issues and recommend improvements Meet or exceed quality, accuracy, and timeliness metrics Partner with Product, Compliance, Finance, Treasury, and Contact Center teams Develop subject-matter expertise in annuity products, systems, and procedures Participate in cross-functional projects and initiatives You have College degree preferred or equivalent industry experience 2+ years of insurance, annuity, or retirement operations experience Working knowledge of annuity products preferred Strong organizational skills and attention to detail Ability to exercise discretion and independent judgment Proficiency in Microsoft Outlook, Word, and Excel preferred A positive, service-oriented mindset and commitment to continuous learning LOCATION This is a hybrid role, requiring three days per week onsite in either Bethlehem, PA or Pittsfield, MA office. Team members must be able to come to campus as needed. Onsite requirements are subject to change based on business needs. TRAVEL No travel is required for this position. Salary Range: $42,830.00 - $64,250.00 The salary range reflected above is a good faith estimate of base pay for the primary location of the position. The salary for this position ultimately will be determined based on the education, experience, knowledge, and abilities of the successful candidate. In addition to salary, this role may also be eligible for annual, sales, or other incentive compensation. Our Promise At Guardian, you’ll have the support and flexibility to achieve your professional and personal goals.  Through skill-building, leadership development and philanthropic opportunities, we provide opportunities to build communities and grow your career, surrounded by diverse colleagues with high ethical standards. Inspire Well-Being As part of Guardian’s Purpose – to inspire well-being – we are committed to offering contemporary, supportive, flexible, and inclusive benefits and resources to our colleagues. Explore our company benefits at www.guardianlife.com/careers/corporate/benefits . Benefits apply to full-time eligible employees. Interns are not eligible for most Company benefits. Equal Employment Opportunity Guardian is an equal opportunity employer. All qualified applicants will be considered for employment without regard to age, race, color, creed, religion, sex, affectional or sexual orientation, national origin, ancestry, marital status, disability, military or veteran status, or any other classification protected by applicable law. Accommodations Guardian is committed to providing access, equal opportunity and reasonable accommodation for individuals with disabilities in employment, its services, programs, and activities. Guardian also provides reasonable accommodations to qualified job applicants (and employees) to accommodate the individual's known limitations related to pregnancy, childbirth, or related medical conditions, unless doing so would create an undue hardship. If reasonable accommodation is needed to participate in the job application or interview process, to perform essential job functions, and/or to receive other benefits and privileges of employment, please contact MyHR@glic.com. Please note: this resource is for accommodation requests only. For all other inquires related to your application and careers at Guardian, refer to the Guardian Careers site. Visa Sponsorship Guardian is not currently or in the foreseeable future sponsoring employment visas.  In order to be a successful applicant. you must be legally authorized to work in the United States, without the need for employer sponsorship. Current Guardian Colleagues: Please apply through the internal Jobs Hub in Workday.</t>
         </is>
       </c>
       <c r="D32" s="3" t="inlineStr">
@@ -1866,7 +1866,11 @@
           <t>Bethlehem</t>
         </is>
       </c>
-      <c r="E32" s="3" t="inlineStr"/>
+      <c r="E32" s="3" t="inlineStr">
+        <is>
+          <t>Pittsfield</t>
+        </is>
+      </c>
       <c r="F32" s="3" t="inlineStr">
         <is>
           <t>2026-02-10</t>
@@ -1874,7 +1878,7 @@
       </c>
       <c r="G32" s="3" t="inlineStr">
         <is>
-          <t>R000108623</t>
+          <t>R000108593</t>
         </is>
       </c>
       <c r="H32" s="3" t="inlineStr">
@@ -1884,7 +1888,7 @@
       </c>
       <c r="I32" s="3" t="inlineStr">
         <is>
-          <t>https://guardianlife.wd5.myworkdayjobs.com/Guardian-Life-Careers/job/Bethlehem/Payroll-Specialist_R000108623</t>
+          <t>https://guardianlife.wd5.myworkdayjobs.com/Guardian-Life-Careers/job/Bethlehem/Annuity-Operations-Care-Specialist_R000108593</t>
         </is>
       </c>
     </row>
@@ -1896,17 +1900,17 @@
       </c>
       <c r="B33" s="4" t="inlineStr">
         <is>
-          <t>Dental Network Support Associate IV</t>
+          <t>Lead, Payroll Specialist</t>
         </is>
       </c>
       <c r="C33" s="4" t="inlineStr">
         <is>
-          <t>As the Dental Network Support Associate IV - Provider Relations team member, you will work directly with contracted providers to help resolve issues, assess and negotiate provider fee schedules, and attempt to reverse termination requests. You will work in a variety of different systems and partner with other network team members. You will also work on different projects related to our dental network providers. “People Count,” “We Do the Right Thing,” and “We Hold Ourselves to Very High Standards” are integral to our team culture. You are A team player with a positive attitude who is self-driven and focused on delivering exceptional results Able to deliver top customer service to all DHMO and PPO dentists and maintain productivity requirements as established by the role Intellectually curious and proactive Displays technical and functional competence and expertise Proactively looks at new and different ways of approaching work You have 3+ years of dental insurance industry experience or comparable insurance experience communicating with Dental or Doctor offices The ability to accelerate impact and drive results Excellent decision making, critical thinking and communication skills Knowledge of Dental or related experience Knowledge of MS Word/Excel/PPT Excellent written and verbal communication skills Bachelor’s Degree or equivalent work experience required You will Assess and analyze provider fee schedules Leverage available data to negotiate mutually beneficial fee schedule increases with providers Research and resolve a variety of provider issues Grow knowledge base of Network strategy Work on a variety of projects Be accountable for meeting contractual and procedural turnaround times Put forth all reasonable efforts to retain providers in the network Provide outstanding customer service to providers and internal partners Location This is a remote role with 0-10% Travel - Travel to/from regional offices as needed for project work/team meeting. Salary Range: $49,260.00 - $73,890.00 The salary range reflected above is a good faith estimate of base pay for the primary location of the position. The salary for this position ultimately will be determined based on the education, experience, knowledge, and abilities of the successful candidate. In addition to salary, this role may also be eligible for annual, sales, or other incentive compensation. Our Promise At Guardian, you’ll have the support and flexibility to achieve your professional and personal goals.  Through skill-building, leadership development and philanthropic opportunities, we provide opportunities to build communities and grow your career, surrounded by diverse colleagues with high ethical standards. Inspire Well-Being As part of Guardian’s Purpose – to inspire well-being – we are committed to offering contemporary, supportive, flexible, and inclusive benefits and resources to our colleagues. Explore our company benefits at www.guardianlife.com/careers/corporate/benefits . Benefits apply to full-time eligible employees. Interns are not eligible for most Company benefits. Equal Employment Opportunity Guardian is an equal opportunity employer. All qualified applicants will be considered for employment without regard to age, race, color, creed, religion, sex, affectional or sexual orientation, national origin, ancestry, marital status, disability, military or veteran status, or any other classification protected by applicable law. Accommodations Guardian is committed to providing access, equal opportunity and reasonable accommodation for individuals with disabilities in employment, its services, programs, and activities. Guardian also provides reasonable accommodations to qualified job applicants (and employees) to accommodate the individual's known limitations related to pregnancy, childbirth, or related medical conditions, unless doing so would create an undue hardship. If reasonable accommodation is needed to participate in the job application or interview process, to perform essential job functions, and/or to receive other benefits and privileges of employment, please contact MyHR@glic.com. Please note: this resource is for accommodation requests only. For all other inquires related to your application and careers at Guardian, refer to the Guardian Careers site. Visa Sponsorship Guardian is not currently or in the foreseeable future sponsoring employment visas.  In order to be a successful applicant. you must be legally authorized to work in the United States, without the need for employer sponsorship. Current Guardian Colleagues: Please apply through the internal Jobs Hub in Workday.</t>
+          <t>Is the opportunity to join a culture where “We Do the Right Thing,” and “We Courageously Shape Our Future Together” important to you? If so, Guardian is seeking a talented and motivated individual to join our team as a Lead, Payroll Specialist. This role will ensure that all payroll administration and accounting processes are regularly evaluated to be as streamlined and efficient as possible. It will be vital to ensure accuracy and timeliness response to ensure an ideal colleague experience across Guardian businesses. You will: Administer payroll for multiple schedules, ensuring timely and accurate compensation for all employees. Maintain payroll controls and procedures to support accuracy and safeguard sensitive information. Assist with wage garnishment vendor management, including processing orders and communicating with vendors. Streamline payroll processes to improve efficiency and reduce errors. Prepare third-party payment requests related to payroll deductions and statutory obligations. Collaborate with related departments to resolve payroll issues and support organizational goals. Serve as a Tier 3 payroll authority by addressing complex payroll questions and escalations. Support accounting functions through accurate payroll reporting and reconciliation. Crosstrain payroll staff to ensure team coverage and continuity of operations. You have: Strong proficiency with Workday Payroll module (required). Knowledge of Workday HCM a plus. Minimum of 4 years of demonstrated experience in payroll functions. Ability to function as a working (hands-on) payroll lead processing payroll, as well as cover for team members in back-up role for vacation and/or high-volume work efforts. Strong focus on customer service, working as a supportive escalation expert to the HR Shared Services Center and a valued partner to other COEs and HR Business Partners as required. Ability to manage sensitive information, working with internal partners to accomplish objectives without compromising a high threshold for discretion and confidentiality. Highly autonomous and self-motivated, demonstrating sound judgment and initiative while keeping others informed as appropriate. Time management skills to successfully prioritize multiple projects at a given time. Strong skills in Microsoft Office applications, especially MS Word and MS Excel. Knowledge of payroll administration, controls, governance, and accounting best practices with established network for keeping current including but not limited to multi-state payroll practices, requirements, and financial/tax implications. Understanding of current federal, state, and local regulatory and compliance obligations related to payroll and how to fulfil them in a timely and accurate manner. Reporting Relationship This position reports to the Head of Payroll who then reports to the Head of HR Service Delivery. Location: Hybrid role: 3 days in Bethlehem, PA office. 2 days WFH. Salary Range: $68,970.00 - $113,310.00 The salary range reflected above is a good faith estimate of base pay for the primary location of the position. The salary for this position ultimately will be determined based on the education, experience, knowledge, and abilities of the successful candidate. In addition to salary, this role may also be eligible for annual, sales, or other incentive compensation. Our Promise At Guardian, you’ll have the support and flexibility to achieve your professional and personal goals.  Through skill-building, leadership development and philanthropic opportunities, we provide opportunities to build communities and grow your career, surrounded by diverse colleagues with high ethical standards. Inspire Well-Being As part of Guardian’s Purpose – to inspire well-being – we are committed to offering contemporary, supportive, flexible, and inclusive benefits and resources to our colleagues. Explore our company benefits at www.guardianlife.com/careers/corporate/benefits . Benefits apply to full-time eligible employees. Interns are not eligible for most Company benefits. Equal Employment Opportunity Guardian is an equal opportunity employer. All qualified applicants will be considered for employment without regard to age, race, color, creed, religion, sex, affectional or sexual orientation, national origin, ancestry, marital status, disability, military or veteran status, or any other classification protected by applicable law. Accommodations Guardian is committed to providing access, equal opportunity and reasonable accommodation for individuals with disabilities in employment, its services, programs, and activities. Guardian also provides reasonable accommodations to qualified job applicants (and employees) to accommodate the individual's known limitations related to pregnancy, childbirth, or related medical conditions, unless doing so would create an undue hardship. If reasonable accommodation is needed to participate in the job application or interview process, to perform essential job functions, and/or to receive other benefits and privileges of employment, please contact MyHR@glic.com. Please note: this resource is for accommodation requests only. For all other inquires related to your application and careers at Guardian, refer to the Guardian Careers site. Visa Sponsorship Guardian is not currently or in the foreseeable future sponsoring employment visas.  In order to be a successful applicant. you must be legally authorized to work in the United States, without the need for employer sponsorship. Current Guardian Colleagues: Please apply through the internal Jobs Hub in Workday.</t>
         </is>
       </c>
       <c r="D33" s="4" t="inlineStr">
         <is>
-          <t>Remote - United States</t>
+          <t>Bethlehem</t>
         </is>
       </c>
       <c r="E33" s="4" t="inlineStr"/>
@@ -1917,17 +1921,17 @@
       </c>
       <c r="G33" s="4" t="inlineStr">
         <is>
-          <t>R000108581</t>
+          <t>R000108623</t>
         </is>
       </c>
       <c r="H33" s="4" t="inlineStr">
         <is>
-          <t>Fully Remote</t>
+          <t>Hybrid - In office 3 days per week</t>
         </is>
       </c>
       <c r="I33" s="4" t="inlineStr">
         <is>
-          <t>https://guardianlife.wd5.myworkdayjobs.com/Guardian-Life-Careers/job/Remote---United-States/Dental-Network-Support-Associate-IV_R000108581</t>
+          <t>https://guardianlife.wd5.myworkdayjobs.com/Guardian-Life-Careers/job/Bethlehem/Payroll-Specialist_R000108623</t>
         </is>
       </c>
     </row>
@@ -1939,24 +1943,20 @@
       </c>
       <c r="B34" s="3" t="inlineStr">
         <is>
-          <t>Senior Data Analyst</t>
+          <t>Dental Network Support Associate IV</t>
         </is>
       </c>
       <c r="C34" s="3" t="inlineStr">
         <is>
-          <t>We are seeking a highly skilled and motivated Senior Data Analyst to join the Enterprise Strategy &amp; Growth Initiatives team. In this role, you will play a crucial part in designing, building, and maintaining the feature engineering pipelines that power our predictive &amp; descriptive data science use cases. Your expertise will help us transform raw data into actionable insights, ensuring that our data solutions are robust, scalable and efficient. The ideal candidate will have a passion for data, thrive in a collaborative environment, and are excited about leveraging cutting-edge technologies to drive business success alongside fellow data analysts, engineers, and scientists. Responsibilities: Design, build and maintain robust &amp; scalable data pipelines to feed descriptive analytics and predictive analytics use cases. Construct meaningful data assets sourced from structured, semi structured, and unstructured data. Ensure data quality, accuracy and integrity of the data assets created. Automate the data pipelines end to end. Participate in data modeling and schema design. Work closely with business stakeholders and data scientists to understand the business process and data needs to translate them into an effective data solution. Collaborate with Stakeholders, Analysts, and Data Scientists to understand the data requirements &amp; deliver optimal solutions (Training, Testing, and Live Scoring) Collaborate with cross-functional teams to identify the right data sources for the use cases. Perform data discovery and analysis on various data sources. Find and tell the compelling narrative of the data that aligns to the intended audience. Create and maintain Data Dictionary for the data pipelines. Participate in code reviews and documentation efforts to maintain high-quality code and data documentation. Qualifications: Bachelor’s degree in STEM related field or equivalent. At least 5 years of experience in Data/Feature/ML Engineering or similar role. Strong understanding of engineering principles, best practices, and software development life cycle. Proficiency in SQL, Python, PySpark and bash scripts. Knowledge of Databricks. Experience with the design and development of ETL/ELT process. Experience working in a Data warehouse. Strong analytical and problem-solving skills. Excellent communication and collaboration skills to work across multiple groups within the organization. Nice to Haves: Experience in the insurance industry Experience working with Data Science Experience working with/creating point-in-time data assets Experience with Databricks Workflows Experience with AWS Tools and Services Location: Three days a week at a Guardian office in Bethlehem, PA or New York, NY. Salary Range: $79,310.00 - $130,295.00 The salary range reflected above is a good faith estimate of base pay for the primary location of the position. The salary for this position ultimately will be determined based on the education, experience, knowledge, and abilities of the successful candidate. In addition to salary, this role may also be eligible for annual, sales, or other incentive compensation. Our Promise At Guardian, you’ll have the support and flexibility to achieve your professional and personal goals.  Through skill-building, leadership development and philanthropic opportunities, we provide opportunities to build communities and grow your career, surrounded by diverse colleagues with high ethical standards. Inspire Well-Being As part of Guardian’s Purpose – to inspire well-being – we are committed to offering contemporary, supportive, flexible, and inclusive benefits and resources to our colleagues. Explore our company benefits at www.guardianlife.com/careers/corporate/benefits . Benefits apply to full-time eligible employees. Interns are not eligible for most Company benefits. Equal Employment Opportunity Guardian is an equal opportunity employer. All qualified applicants will be considered for employment without regard to age, race, color, creed, religion, sex, affectional or sexual orientation, national origin, ancestry, marital status, disability, military or veteran status, or any other classification protected by applicable law. Accommodations Guardian is committed to providing access, equal opportunity and reasonable accommodation for individuals with disabilities in employment, its services, programs, and activities. Guardian also provides reasonable accommodations to qualified job applicants (and employees) to accommodate the individual's known limitations related to pregnancy, childbirth, or related medical conditions, unless doing so would create an undue hardship. If reasonable accommodation is needed to participate in the job application or interview process, to perform essential job functions, and/or to receive other benefits and privileges of employment, please contact MyHR@glic.com. Please note: this resource is for accommodation requests only. For all other inquires related to your application and careers at Guardian, refer to the Guardian Careers site. Visa Sponsorship Guardian is not currently or in the foreseeable future sponsoring employment visas.  In order to be a successful applicant. you must be legally authorized to work in the United States, without the need for employer sponsorship. Current Guardian Colleagues: Please apply through the internal Jobs Hub in Workday.</t>
+          <t>As the Dental Network Support Associate IV - Provider Relations team member, you will work directly with contracted providers to help resolve issues, assess and negotiate provider fee schedules, and attempt to reverse termination requests. You will work in a variety of different systems and partner with other network team members. You will also work on different projects related to our dental network providers. “People Count,” “We Do the Right Thing,” and “We Hold Ourselves to Very High Standards” are integral to our team culture. You are A team player with a positive attitude who is self-driven and focused on delivering exceptional results Able to deliver top customer service to all DHMO and PPO dentists and maintain productivity requirements as established by the role Intellectually curious and proactive Displays technical and functional competence and expertise Proactively looks at new and different ways of approaching work You have 3+ years of dental insurance industry experience or comparable insurance experience communicating with Dental or Doctor offices The ability to accelerate impact and drive results Excellent decision making, critical thinking and communication skills Knowledge of Dental or related experience Knowledge of MS Word/Excel/PPT Excellent written and verbal communication skills Bachelor’s Degree or equivalent work experience required You will Assess and analyze provider fee schedules Leverage available data to negotiate mutually beneficial fee schedule increases with providers Research and resolve a variety of provider issues Grow knowledge base of Network strategy Work on a variety of projects Be accountable for meeting contractual and procedural turnaround times Put forth all reasonable efforts to retain providers in the network Provide outstanding customer service to providers and internal partners Location This is a remote role with 0-10% Travel - Travel to/from regional offices as needed for project work/team meeting. Salary Range: $49,260.00 - $73,890.00 The salary range reflected above is a good faith estimate of base pay for the primary location of the position. The salary for this position ultimately will be determined based on the education, experience, knowledge, and abilities of the successful candidate. In addition to salary, this role may also be eligible for annual, sales, or other incentive compensation. Our Promise At Guardian, you’ll have the support and flexibility to achieve your professional and personal goals.  Through skill-building, leadership development and philanthropic opportunities, we provide opportunities to build communities and grow your career, surrounded by diverse colleagues with high ethical standards. Inspire Well-Being As part of Guardian’s Purpose – to inspire well-being – we are committed to offering contemporary, supportive, flexible, and inclusive benefits and resources to our colleagues. Explore our company benefits at www.guardianlife.com/careers/corporate/benefits . Benefits apply to full-time eligible employees. Interns are not eligible for most Company benefits. Equal Employment Opportunity Guardian is an equal opportunity employer. All qualified applicants will be considered for employment without regard to age, race, color, creed, religion, sex, affectional or sexual orientation, national origin, ancestry, marital status, disability, military or veteran status, or any other classification protected by applicable law. Accommodations Guardian is committed to providing access, equal opportunity and reasonable accommodation for individuals with disabilities in employment, its services, programs, and activities. Guardian also provides reasonable accommodations to qualified job applicants (and employees) to accommodate the individual's known limitations related to pregnancy, childbirth, or related medical conditions, unless doing so would create an undue hardship. If reasonable accommodation is needed to participate in the job application or interview process, to perform essential job functions, and/or to receive other benefits and privileges of employment, please contact MyHR@glic.com. Please note: this resource is for accommodation requests only. For all other inquires related to your application and careers at Guardian, refer to the Guardian Careers site. Visa Sponsorship Guardian is not currently or in the foreseeable future sponsoring employment visas.  In order to be a successful applicant. you must be legally authorized to work in the United States, without the need for employer sponsorship. Current Guardian Colleagues: Please apply through the internal Jobs Hub in Workday.</t>
         </is>
       </c>
       <c r="D34" s="3" t="inlineStr">
         <is>
-          <t>Bethlehem</t>
-        </is>
-      </c>
-      <c r="E34" s="3" t="inlineStr">
-        <is>
-          <t>New York</t>
-        </is>
-      </c>
+          <t>Remote - United States</t>
+        </is>
+      </c>
+      <c r="E34" s="3" t="inlineStr"/>
       <c r="F34" s="3" t="inlineStr">
         <is>
           <t>2026-02-10</t>
@@ -1964,17 +1964,17 @@
       </c>
       <c r="G34" s="3" t="inlineStr">
         <is>
-          <t>R000108281</t>
+          <t>R000108581</t>
         </is>
       </c>
       <c r="H34" s="3" t="inlineStr">
         <is>
-          <t>Hybrid - In office 3 days per week</t>
+          <t>Fully Remote</t>
         </is>
       </c>
       <c r="I34" s="3" t="inlineStr">
         <is>
-          <t>https://guardianlife.wd5.myworkdayjobs.com/Guardian-Life-Careers/job/Bethlehem/Senior-Data-Analyst_R000108281</t>
+          <t>https://guardianlife.wd5.myworkdayjobs.com/Guardian-Life-Careers/job/Remote---United-States/Dental-Network-Support-Associate-IV_R000108581</t>
         </is>
       </c>
     </row>
@@ -1984,14 +1984,46 @@
           <t>2026-02-25</t>
         </is>
       </c>
-      <c r="B35" s="4" t="inlineStr"/>
-      <c r="C35" s="4" t="inlineStr"/>
-      <c r="D35" s="4" t="inlineStr"/>
-      <c r="E35" s="4" t="inlineStr"/>
-      <c r="F35" s="4" t="inlineStr"/>
-      <c r="G35" s="4" t="inlineStr"/>
-      <c r="H35" s="4" t="inlineStr"/>
-      <c r="I35" s="4" t="inlineStr"/>
+      <c r="B35" s="4" t="inlineStr">
+        <is>
+          <t>Senior Data Analyst</t>
+        </is>
+      </c>
+      <c r="C35" s="4" t="inlineStr">
+        <is>
+          <t>We are seeking a highly skilled and motivated Senior Data Analyst to join the Enterprise Strategy &amp; Growth Initiatives team. In this role, you will play a crucial part in designing, building, and maintaining the feature engineering pipelines that power our predictive &amp; descriptive data science use cases. Your expertise will help us transform raw data into actionable insights, ensuring that our data solutions are robust, scalable and efficient. The ideal candidate will have a passion for data, thrive in a collaborative environment, and are excited about leveraging cutting-edge technologies to drive business success alongside fellow data analysts, engineers, and scientists. Responsibilities: Design, build and maintain robust &amp; scalable data pipelines to feed descriptive analytics and predictive analytics use cases. Construct meaningful data assets sourced from structured, semi structured, and unstructured data. Ensure data quality, accuracy and integrity of the data assets created. Automate the data pipelines end to end. Participate in data modeling and schema design. Work closely with business stakeholders and data scientists to understand the business process and data needs to translate them into an effective data solution. Collaborate with Stakeholders, Analysts, and Data Scientists to understand the data requirements &amp; deliver optimal solutions (Training, Testing, and Live Scoring) Collaborate with cross-functional teams to identify the right data sources for the use cases. Perform data discovery and analysis on various data sources. Find and tell the compelling narrative of the data that aligns to the intended audience. Create and maintain Data Dictionary for the data pipelines. Participate in code reviews and documentation efforts to maintain high-quality code and data documentation. Qualifications: Bachelor’s degree in STEM related field or equivalent. At least 5 years of experience in Data/Feature/ML Engineering or similar role. Strong understanding of engineering principles, best practices, and software development life cycle. Proficiency in SQL, Python, PySpark and bash scripts. Knowledge of Databricks. Experience with the design and development of ETL/ELT process. Experience working in a Data warehouse. Strong analytical and problem-solving skills. Excellent communication and collaboration skills to work across multiple groups within the organization. Nice to Haves: Experience in the insurance industry Experience working with Data Science Experience working with/creating point-in-time data assets Experience with Databricks Workflows Experience with AWS Tools and Services Location: Three days a week at a Guardian office in Bethlehem, PA or New York, NY. Salary Range: $79,310.00 - $130,295.00 The salary range reflected above is a good faith estimate of base pay for the primary location of the position. The salary for this position ultimately will be determined based on the education, experience, knowledge, and abilities of the successful candidate. In addition to salary, this role may also be eligible for annual, sales, or other incentive compensation. Our Promise At Guardian, you’ll have the support and flexibility to achieve your professional and personal goals.  Through skill-building, leadership development and philanthropic opportunities, we provide opportunities to build communities and grow your career, surrounded by diverse colleagues with high ethical standards. Inspire Well-Being As part of Guardian’s Purpose – to inspire well-being – we are committed to offering contemporary, supportive, flexible, and inclusive benefits and resources to our colleagues. Explore our company benefits at www.guardianlife.com/careers/corporate/benefits . Benefits apply to full-time eligible employees. Interns are not eligible for most Company benefits. Equal Employment Opportunity Guardian is an equal opportunity employer. All qualified applicants will be considered for employment without regard to age, race, color, creed, religion, sex, affectional or sexual orientation, national origin, ancestry, marital status, disability, military or veteran status, or any other classification protected by applicable law. Accommodations Guardian is committed to providing access, equal opportunity and reasonable accommodation for individuals with disabilities in employment, its services, programs, and activities. Guardian also provides reasonable accommodations to qualified job applicants (and employees) to accommodate the individual's known limitations related to pregnancy, childbirth, or related medical conditions, unless doing so would create an undue hardship. If reasonable accommodation is needed to participate in the job application or interview process, to perform essential job functions, and/or to receive other benefits and privileges of employment, please contact MyHR@glic.com. Please note: this resource is for accommodation requests only. For all other inquires related to your application and careers at Guardian, refer to the Guardian Careers site. Visa Sponsorship Guardian is not currently or in the foreseeable future sponsoring employment visas.  In order to be a successful applicant. you must be legally authorized to work in the United States, without the need for employer sponsorship. Current Guardian Colleagues: Please apply through the internal Jobs Hub in Workday.</t>
+        </is>
+      </c>
+      <c r="D35" s="4" t="inlineStr">
+        <is>
+          <t>Bethlehem</t>
+        </is>
+      </c>
+      <c r="E35" s="4" t="inlineStr">
+        <is>
+          <t>New York</t>
+        </is>
+      </c>
+      <c r="F35" s="4" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="G35" s="4" t="inlineStr">
+        <is>
+          <t>R000108281</t>
+        </is>
+      </c>
+      <c r="H35" s="4" t="inlineStr">
+        <is>
+          <t>Hybrid - In office 3 days per week</t>
+        </is>
+      </c>
+      <c r="I35" s="4" t="inlineStr">
+        <is>
+          <t>https://guardianlife.wd5.myworkdayjobs.com/Guardian-Life-Careers/job/Bethlehem/Senior-Data-Analyst_R000108281</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
@@ -2226,14 +2258,46 @@
           <t>2026-02-25</t>
         </is>
       </c>
-      <c r="B41" s="4" t="inlineStr"/>
-      <c r="C41" s="4" t="inlineStr"/>
-      <c r="D41" s="4" t="inlineStr"/>
-      <c r="E41" s="4" t="inlineStr"/>
-      <c r="F41" s="4" t="inlineStr"/>
-      <c r="G41" s="4" t="inlineStr"/>
-      <c r="H41" s="4" t="inlineStr"/>
-      <c r="I41" s="4" t="inlineStr"/>
+      <c r="B41" s="4" t="inlineStr">
+        <is>
+          <t>Lead Data Engineer</t>
+        </is>
+      </c>
+      <c r="C41" s="4" t="inlineStr">
+        <is>
+          <t>Guardian is seeking a highly skilled and motivated Lead Data Engineer to join the FPRS&amp;CSWM Data Engineering team. In this role, you will play a crucial part in designing, building, and maintaining the data pipelines that power our Operational ,reporting, ML &amp; AI use cases. Your expertise will help us transform raw data into actionable insights via data products, ensuring that our data solutions are robust, scalable and efficient. The ideal candidate will have a passion for data engineering, thrive in a collaborative environment and are excited about leveraging cutting-edge technologies to drive business success. Your contributions will go beyond hands-on engineering, as you help bring life to innovative ideas and mentor other engineers. You’ll thrive in a fast-paced, collaborative environment, balancing technical execution with a deep understanding of business needs. We value curiosity, creativity, and continuous learning. If you’re passionate about solving meaningful problems and creating value through data-driven innovation, we look forward to welcoming you to our team. You will Lead technical design and implementation of data engineering solutions, ensuring best practices and high-quality deliverables. Mentor and guide junior engineers, conducting code reviews and technical sessions to foster team growth. Perform detailed analysis of raw data sources by applying business context and collaborate with cross-functional teams to transform raw data into data products Create scalable and trusted data pipelines which generate curated data assets in centralized data lake/data warehouse ecosystems. Monitor and troubleshoot data pipeline performance, identifying and resolving bottlenecks and issues. Construct meaningful data assets sourced from structured, semi structured, and unstructured data. Develop real-time data solutions by creating new API endpoints or streaming frameworks. Develop, test, and maintain robust tools, frameworks, and libraries that standardize and streamline the data lifecycle. Collaborate with cross-functional teams of Data Science, Data Engineering, business units, and other IT teams. Create and maintain effective documentation for projects and practices, ensuring transparency and effective team communication. Provide technical leadership and mentorship on continuous improvement in building reusable and scalable solutions. Contribute to enhancing strategy for advanced data engineering practices and lead execution of key initiatives. Stay up-to-date with the latest trends in modern data engineering, machine learning &amp; AI. You have Bachelor’s or Master’s degree with 8+ years of experience in Computer Science, Engineering, or a related field. 5+ years of experience working with Python, SQL, PySpark, and bash scripts. Proficient in software development lifecycle and software engineering practices. 4+ years of experience developing and maintaining robust data pipelines for both structured and unstructured data for advanced analytical and reporting use cases. 3+ years of experience working with Cloud Data Warehousing (Redshift, Snowflake, Databricks SQL or equivalent) platforms and distributed frameworks like Spark. 2+ years of experience leading a team of engineers and a track record of delivering robust and scalable data solutions with highest quality. Solid understanding of data modeling and warehousing techniques. Experience working in a data warehouse is a plus. Proficiency in understanding REST APIs, experience using different types of APIs to extract data or perform functionalities. Hands-on experience building and maintaining tools and libraries used by multiple teams across the organization (e.g., Data Engineering utility libraries, DQ Libraries). Proficient in understanding and incorporating software engineering principles in design &amp; development process. Hands-on experience with CI/CD tools (e.g., Jenkins or equivalent), version control (Github, Bitbucket), orchestration (Airflow, Prefect or equivalent). Excellent communication skills and ability to work and collaborate with cross-functional teams across technology and business. Location Three days a week at a Guardian office in Bethlehem, PA, New York, NY. Pittsfield, MA or Holmdel, NJ. Salary Range: $99,150.00 - $162,885.00 The salary range reflected above is a good faith estimate of base pay for the primary location of the position. The salary for this position ultimately will be determined based on the education, experience, knowledge, and abilities of the successful candidate. In addition to salary, this role may also be eligible for annual, sales, or other incentive compensation. Our Promise At Guardian, you’ll have the support and flexibility to achieve your professional and personal goals.  Through skill-building, leadership development and philanthropic opportunities, we provide opportunities to build communities and grow your career, surrounded by diverse colleagues with high ethical standards. Inspire Well-Being As part of Guardian’s Purpose – to inspire well-being – we are committed to offering contemporary, supportive, flexible, and inclusive benefits and resources to our colleagues. Explore our company benefits at www.guardianlife.com/careers/corporate/benefits . Benefits apply to full-time eligible employees. Interns are not eligible for most Company benefits. Equal Employment Opportunity Guardian is an equal opportunity employer. All qualified applicants will be considered for employment without regard to age, race, color, creed, religion, sex, affectional or sexual orientation, national origin, ancestry, marital status, disability, military or veteran status, or any other classification protected by applicable law. Accommodations Guardian is committed to providing access, equal opportunity and reasonable accommodation for individuals with disabilities in employment, its services, programs, and activities. Guardian also provides reasonable accommodations to qualified job applicants (and employees) to accommodate the individual's known limitations related to pregnancy, childbirth, or related medical conditions, unless doing so would create an undue hardship. If reasonable accommodation is needed to participate in the job application or interview process, to perform essential job functions, and/or to receive other benefits and privileges of employment, please contact MyHR@glic.com. Please note: this resource is for accommodation requests only. For all other inquires related to your application and careers at Guardian, refer to the Guardian Careers site. Visa Sponsorship Guardian is not currently or in the foreseeable future sponsoring employment visas.  In order to be a successful applicant. you must be legally authorized to work in the United States, without the need for employer sponsorship. Current Guardian Colleagues: Please apply through the internal Jobs Hub in Workday.</t>
+        </is>
+      </c>
+      <c r="D41" s="4" t="inlineStr">
+        <is>
+          <t>Bethlehem</t>
+        </is>
+      </c>
+      <c r="E41" s="4" t="inlineStr">
+        <is>
+          <t>New York, Pittsfield, Holmdel</t>
+        </is>
+      </c>
+      <c r="F41" s="4" t="inlineStr">
+        <is>
+          <t>2026-02-05</t>
+        </is>
+      </c>
+      <c r="G41" s="4" t="inlineStr">
+        <is>
+          <t>R000108510</t>
+        </is>
+      </c>
+      <c r="H41" s="4" t="inlineStr">
+        <is>
+          <t>Hybrid - In office 3 days per week</t>
+        </is>
+      </c>
+      <c r="I41" s="4" t="inlineStr">
+        <is>
+          <t>https://guardianlife.wd5.myworkdayjobs.com/Guardian-Life-Careers/job/Bethlehem/Lead-Data-Engineer_R000108510</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="inlineStr">

</xml_diff>